<commit_message>
export feather and csv
</commit_message>
<xml_diff>
--- a/data/excelfiles/df_neuheiten_blatter.xlsx
+++ b/data/excelfiles/df_neuheiten_blatter.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,2384 +436,2415 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>Titel</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>untertitel</t>
+          <t>Preis</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>autor</t>
+          <t>Autor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>verlag</t>
+          <t>Genre</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>preis</t>
+          <t>Text</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>seiten</t>
+          <t>ISBN/GTIN</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sprache</t>
+          <t>Produktart</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>einband</t>
+          <t>Einbandart</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>erscheinungsjahr</t>
+          <t>Verlag</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>artikelnummer</t>
+          <t>Erscheinungsdatum</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>isbn</t>
+          <t>Auflage</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>auflage</t>
+          <t>Reihe</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>reihe</t>
+          <t>Seiten</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>reihenbandnummer</t>
+          <t>Sprache</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Masse</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Artikel-Nr.</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Die spürst du nicht </t>
+          <t>Der Feind</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>24.90</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Glattauer, Daniel</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Zsolnay</t>
-        </is>
-      </c>
+          <t>Brand, Christine</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CHF 34.50</t>
+          <t>Ein bizarre Mordserie an Männern sowie Schüsse während einer Frauendisko - in Band 5 der Erfolgsserie halten gleich zwei Fälle Milla Nova und das Team um Sandro Bandini auf Trab.
+Ein bizarrer Mord sorgt für Aufsehen: Ein Mann wurde an sein Bett gefesselt und hingerichtet. An den Füßen trägt er rote Stöckelschuhe. Schnell stellt sich heraus, dass er zuvor eine Drohung erhielt: ein Foto von sich selbst - mit dem Absatz eines Stöckelschuhs im Gesicht. Er ist nicht der Einzige, der solch eine Nachricht bekam. Sind auch die anderen Bedrohten in Gefahr? Gleichzeitig jagt das Team um Polizeichef Sandro Bandini einen Mann, der in einer Frauendisko in einem linken Kulturzentrum um sich schoss. Die Vermutung eines rechtsextremen Hintergrunds liegt nahe, doch TV-Reporterin Milla Nova vermutet ein anderes Motiv: Frauenhass. Gemeinsam mit ihrem blinden Freund Nathaniel taucht sie in die dunkle Welt der Incels ein. Zwei Fälle, bei denen der Hass auf das andere Geschlecht eine vitale Rolle spielt. Ist es Zufall oder besteht ein Zusammenhang?
+Die unabhängig voneinander lesbaren Krimis um Milla Nova und Sandro Bandini:
+1. Blind
+2. Die Patientin
+3. Der Bruder
+4. Der Unbekannte
+5. Der Feind
+Lesen Sie auch »Wahre Verbrechen»: Christine Brand schreibt über ihre dramatischsten Fälle als Gerichtsreporterin.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>304 S.</t>
+          <t>978-3-7645-0771-8</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>42421530</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>978-3-552-07333-3</t>
+          <t>1. A.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.05</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Der Bestsellerautor Daniel Glattauer lässt in seinem neuen Roman Menschen zu Wort kommen, die keine Stimme haben - ein Sittenbild unserer privilegierten Gesellschaft. Die Binders und die Strobl-Marineks gönnen sich einen exklusiven Urlaub in der Toskana. Tochter Sophie Luise, 14, durfte gegen die Langeweile ihre Schulfreundin Aayana mitnehmen, ein Flüchtlingskind aus Somalia. Kaum hat man sich mit Prosecco und Antipasti in Ferienlaune gechillt, kommt es zur Katastrophe. Was ist ein Menschenleben wert? Und jedes gleich viel? Daniel Glattauer packt große Fragen in seinen neuen Roman, den man nicht mehr aus der Hand legen kann und in dem er all sein Können ausspielt: spannende Szenen, starke Dialoge, Sprachwitz. Dabei zeichnet Glattauer ein Sittenbild unserer privilegierten Gesellschaft, entlarvt deren Doppelmoral und leiht jenen seine Stimme, die viel zu selten zu Wort kommen.</t>
-        </is>
-      </c>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Besser allein als in schlechter Gesellschaft </t>
+          <t>Die Krume Brot</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Meine eigensinnige Tante</t>
+          <t>29.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Altaras, Adriana</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Kiepenheuer &amp; Witsch</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CHF 30.50</t>
+          <t>Adelina, Tochter italienischer Einwanderer, arbeitet in einer Zürcher Fabrik, als sie nach kurzem Liebesglück mit einem Kind allein dasteht. Sie verliert die Stelle, die Wohnung, kämpft ums Überleben. In der größten Not lernt sie Emil kennen, einen erfolgreichen Grafiker, der ihre Schulden bezahlt und Adelina mit der kleinen Emma bei sich aufnimmt. Außer an der Liebe fehlt es an nichts. Emil kauft ein Anwesen in den Bergen des Piemont und scheint auf gemeinsames Glück zu hoffen. Aber dann verschwindet das Kind, spurlos.
+Adelina macht sich auf die Suche, begleitet von einem schweigsamen Unbekannten. Er bringt sie nach Mailand, in eine Kommune, zu Menschen, die an die Revolution glauben und Adelina versprechen, die verlorene Tochter zu finden; sie muss nur bereit sein, sich dem Kampf anzuschließen, und mit ihren Schweizer Papieren über die Grenze gehen, auf eine gefährliche Mission.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>240 S.</t>
+          <t>978-3-498-00320-3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Rowohlt</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>42779017</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>978-3-462-00424-3</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Adriana Altaras erzählt von ihrer Tante, der schönen Teta Jele. Von einer Frau, die 101 Jahre alt wurde, die spanische Grippe, das KZ und ihre norditalienische Schwiegermutter überlebte. Von einer so liebevollen wie eigensinnigen Beziehung. Und davon, wie man lernt, das Leben anzunehmen.</t>
-        </is>
-      </c>
+          <t>Breite 133 mm, Höhe 209 mm, Dicke 23 mmGewicht330 g</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sommerschwestern - Die Nacht der Lichter </t>
+          <t>Der Magier im Kreml</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>36.90</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Peetz, Monika</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Kiepenheuer &amp; Witsch</t>
-        </is>
-      </c>
+          <t>Da Empoli, GiulianoMeßner, MichaelaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CHF 23.90</t>
+          <t>SPIEGEL-BESTSELLER UND VIELFACH AUSGEZEICHNET
+Man nennt ihn den «Magier im Kreml». Der rätselhafte Vadim Baranow war Regisseur und Produzent von Reality-TV-Shows, bevor er zur grauen Eminenz von Putin wird. Nachdem er als politischer Berater von der Bühne verschwindet, werden immer mehr Legenden über ihn verbreitet. Bis er eines Nachts dem Ich-Erzähler dieses Buches, der seit Langem in Moskauer Archiven forscht, seine Geschichte anvertraut â¦
+Dieser Roman führt uns ins Zentrum der russischen Macht, wo permanent Intrigen gesponnen werden. Und wo Vadim, der zum wichtigsten Spindoktor des Regimes geworden ist, ein ganzes Land in ein politisches Theater verwandelt, in dem es keine andere Realität als die Erfüllung der Wünsche des Präsidenten gibt. Doch Vadim ist kein gewöhnlicher Ehrgeizling: Der Regisseur, der sich unter die Wölfe verirrt hat, gerät immer tiefer in die Machenschaften des Systems, das er selbst mit aufgebaut hat, und wird alles daransetzen, um dort wieder herauszukommen. Er nimmt den Erzähler mit auf eine Reise ins Herz der Finsternis. «Der Magier im Kreml» ist ein großer Roman über das zeitgenössische Russland und die Entstehung seiner medial inszenierten und vollkommen fiktiven, aber auch tödlichen Realität, einem Imperium der Lüge. Er enthüllt nicht nur die Hintergründe der Putin-Ära, sondern bietet auch eine hellsichtige Betrachtung über die Macht.
+Ausgezeichnet mit dem Grand Prix du Roman de l Académie française
+Finalist des Prix Goncourt 2022
+200 000 verkaufte Exemplare, Platz 1 der Bestenliste in Frankreich
+Die Rechte wurden bereits in 26 Länder verkauft
+Ein Roman über den einflussreichsten Berater von Putin und die mediale Inszenierung der Macht
+Basiert auf der realen Gestalt von Putins Spindoktor Wladislaw Surkow</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>352 S.</t>
+          <t>978-3-406-79993-8</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Beck</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>42779092</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>978-3-462-00398-7</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Die Sommerschwestern-Romane</t>
-        </is>
-      </c>
+          <t>24.04.2023</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Monika Peetz' vier »Sommerschwestern« kehren zurück an ihren Ferienort Bergen an der holländischen Nordseeküste, auf der Spur des großen Familiengeheimnisses. Eine spannende Suche nach der Wahrheit über den Tod ihres Vaters vor sommerlicher Urlaubskulisse. </t>
+          <t>Breite 139 mm, Höhe 217 mm, Dicke 25 mmGewicht480 g</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>55652787</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Der heutige Tag </t>
+          <t>Wo wir uns trafen</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ein Stundenbuch der Liebe</t>
+          <t>32.90</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Schubert, Helga</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>DTV</t>
-        </is>
-      </c>
+          <t>Lundberg, SofiaDörries, MaikeÜbersetzungSchöps, KerstinÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CHF 32.90</t>
+          <t>Nur wahre Freundschaft berührt dein Herz ...
+Lidingö, Südschweden: Jeden zweiten Samstag sitzt die frisch geschiedene Esther auf einer Bank unter einer alten Eiche und schaut hinaus aufs Meer. Die Wochenenden, die ihr Sohn bei seinem Vater verbringt, sind schwer, und hier kann Esther ihren Gefühlen freien Lauf lassen. Eines Tages trifft sie dort auf Rut, eine alleinstehende, ältere Dame, die Esther mit ihrer warmherzigen Art tröstet. Zwischen den beiden Frauen entsteht eine tiefe Freundschaft, und die Bank am Meer wird zu ihrem regelmäßigen Treffpunkt. Doch dann verschwindet Rut, und als Esther sich auf die Suche nach ihr macht, kommt sie einer dramatischen Lebensgeschichte auf die Spur ...</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>272 S.</t>
+          <t>978-3-442-31645-8</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>42827274</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>978-3-423-28319-9</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>»Vielleicht ist einer von uns morgen schon nicht mehr da.«</t>
-        </is>
-      </c>
+          <t>Breite 148 mm, Höhe 221 mm, Dicke 37 mmGewicht564 g</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Der große Preis von Schmonaco </t>
+          <t>Going Zero</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ein Roman aus der Welt von Minecraft FREEDOM von Paluten, Band 6</t>
+          <t>34.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Paluten / Kern, Klaas (Zus. mit) / Zinner, Irina (Illustr.)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Community Editions</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CHF 21.50</t>
+          <t>Hat man als Einzelner überhaupt eine Chance gegen das System? Eine junge Bibliothekarin aus Boston ist entschlossen, es zu versuchen - ihr bleibt keine Wahl. Und so greift sie zu, als sich die Einladung zu einem ungewöhnlichen Kräftemessen bietet: dem Betatest von FUSION, einem Projekt der US-Geheimdienste und des Social-Media-Moguls Cy Baxter. Wem es gelingt, 30 Tage unauffindbar zu bleiben, dem winken 3 Millionen Dollar. Doch Kaitlyn geht es um etwas anderes.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>220 S.</t>
+          <t>978-3-257-07192-4</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>42874349</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>978-3-96096-961-7</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>1. Aufl. 2023</t>
-        </is>
-      </c>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Ein Roman aus der Welt von Minecraft FREEDOM</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Achtung - anschnallen! Im neuen FREEDOM-Band wird Paluten zum Rennfahrer Paluten ist einer der meistgeklickten YouTuber und entertaint Gaming-affine Kids ab 10 Jahren mit seinen witzigen Videos. In seinen beliebten Romanen erlebt er coole Abenteuer in der Welt von FREEDOM. Nach "Die Schmahamas-Verschwörung", "Schlamassel im Weltall", "Donnerwetter am Mount Schmeverest", "Reise zum Mittelschlund der Erde" und "Verschollen im Berschmudadreieck" nimmt Paluten nun am großen Preis von Schmonaco teil.</t>
-        </is>
-      </c>
+          <t>Breite 116 mm, Höhe 184 mm, Dicke 30 mmGewicht403 g</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bündner Sturm </t>
+          <t>Sommernächte in Paris</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ein Fall für Giulia de Medici</t>
+          <t>16.90</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Gurt, Philipp</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Kampa Verlag</t>
-        </is>
-      </c>
+          <t>Swan, KarenWittich, GertrudÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CHF 24.90</t>
+          <t>Ein unvergesslicher Sommer in der Stadt der Liebe ...
+Die Kunstagentin Flora Sykes ist ständig in der Welt unterwegs. Für ein Privatleben oder eine ernsthafte Beziehung bleibt da keine Zeit. Nun führt sie ein geheimnisvoller Auftrag nach Paris, wo die wohlhabende Familie Vermeil ein Apartment voller Kunstschätze geerbt hat, das seit über siebzig Jahren niemand mehr betreten hat. Warum war es so lange verschlossen? Und woher stammen die Bilder? Statt Antworten zu finden, stößt Flora bei ihren Nachforschungen auf immer mehr Geheimnisse. Und zu allem Überfluss lenkt Xavier Vermeil, der unverschämt gut aussehende Sohn der Erben, sie immer wieder von der Arbeit ab ...</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>336 S.</t>
+          <t>978-3-442-49396-8</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>42907560</t>
+          <t>20.04.2023</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>978-3-311-12060-5</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Ein Fall für Giulia de Medici</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>06</t>
-        </is>
-      </c>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Ein Sturm zieht über das herbstlich gefärbte Engadin, als Giulia de Medici, Alpinpolizistin und Chefermittlerin der Kantonspolizei Graubünden, zu einer Leiche auf den Roseggletscher gerufen wird. Dort angekommen, ist Giulias Verwunderung groß: Die fast gänzlich eingefrorene Tote trägt ein rotes Sommerkleid, und die zum Fundort gerufene Forensikerin stellt fest, dass die junge Frau bereits vor über zwanzig Jahren ermordet wurde. Als Giulia auf dem Weg zurück ins Tal in der Berghütte Chamanna Coaz Rast macht und dabei auch noch auf die tote Hüttenwartin stößt, beginnt eine aufreibende Jagd nach den Schuldigen. Liebe, Verrat, Leidenschaft und Intrigen zwingen die temperamentvolle Berglerin beinahe in die Knie.</t>
-        </is>
-      </c>
+          <t>Breite 126 mm, Höhe 187 mm, Dicke 35 mmGewicht394 g</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">°C - Celsius </t>
+          <t>One of the Girls</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thriller - Der neue Bestseller vom Blackout-Autor</t>
+          <t>24.90</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Elsberg, Marc</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Blanvalet</t>
-        </is>
-      </c>
+          <t>Clarke, LucyHofstetter, UrbanÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CHF 35.50</t>
+          <t>Sechs Frauen. Sechs Geheimnisse. Eine Leiche.
+Es sollte der perfekte Kurzurlaub werden: Lexi reist mit fünf Freundinnen auf eine griechische Insel, um ihren Junggesellinnenabschied zu feiern. Von der abgelegenen Villa mit Meerblick bis hin zu den malerischen Tavernen und weiß getünchten Straßen scheint der Urlaub zu schön, um wahr zu sein. Und tatsächlich bekommt die Idylle bald Risse, denn abgesehen von ihrer Freundschaft mit Lexi haben die Frauen nur eines gemeinsam: Sie alle haben etwas zu verbergen. Nach und nach kommen versteckte Absichten ans Licht, Geheimnisse werden enthüllt und die Masken fallen - bis eine Leiche auf den Klippen unterhalb der Villa liegt...</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>608 S.</t>
+          <t>978-3-423-26359-7</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>DTV</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>42939970</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>978-3-7645-0633-9</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>1. A.</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Wenn Sie das Klima beeinflussen könnten, wen würden Sie vor der Erderwärmung retten? Ihre Heimat? Grönland? Afrika?</t>
-        </is>
-      </c>
+          <t>Breite 136 mm, Höhe 210 mm, Dicke 31 mmGewicht450 g</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Feinde </t>
+          <t>Liebe oder Eierlikör - Fast eine Romanze</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>23.90</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Grisham, John / Reiter, Bea (Übers.) / Walsh-Araya, Imke (Übers.)</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Heyne</t>
-        </is>
-      </c>
+          <t>Heldt, Dora</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CHF 32.90</t>
+          <t>Früher war mehr Romantik ...
+Ernst Mannsen versteht die Welt nicht mehr. Die sonst so verlässliche Hilke Petersen trägt plötzlich Lippenstift und hat keine Zeit, auf dem Frühlingsbazar Kuchen zu verkaufen. Hella und Gudrun reden von Frühlingsgefühlen und Liebeshormonen und vermuten, dass Hilke eine Romanze hat. Und plötzlich taucht auch noch das Gerücht auf, dass das halbe Dorf sich bei einer Dating-App angemeldet hat, die Liebe oder Eierlikör heißt. Und das, obwohl Ernst schon so viel über Betrüger im Netz gelesen hat. Er vermutet, dass der Lippenstift nur der Anfang der Katastrophe ist, in die Hilke sich begibt, und ist entschlossen, das zu verhindern. Mithilfe seines Enkels Mats und Freundin Hella forscht er undercover nach, nicht ahnend, wie schnell man sich auf einem Date wiederfinden kann ...</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>544 S.</t>
+          <t>978-3-423-28337-3</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>DTV</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>42940181</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>978-3-453-27420-4</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Biloxi, Mississippi: Die Einwanderersöhne Keith und Hugh wachsen in den Sechzigerjahren gemeinsam auf, verbunden durch eine scheinbar unverbrüchliche Freundschaft. Bis sie sich auf den verschiedenen Seiten des Gesetzes wiederfinden: Keith hat Jura studiert und ist Staatsanwalt geworden. Hugh dagegen arbeitet für seinen Vater, einen Boss der Dixie-Mafia. Eine tödliche Feindschaft entsteht, die vor Gericht ein dramatisches Finale findet.</t>
-        </is>
-      </c>
+          <t>Breite 119 mm, Höhe 175 mm, Dicke 24 mmGewicht280 g</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Windhauch, das ist alles Windhauch </t>
+          <t>Damals im Tessin</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>26.90</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ryser, Werner</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Cosmos</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CHF 36.00</t>
+          <t>Zwanzig Jahre sind vergangen, seit Malvaglia, ein kleines Dorf in den Tessiner Bergen, geflutet wurde, um auf dem Gelände einen Stausee entstehen zu lassen. Beinahe haben die einstigen Bewohner, deren Häuser damals unter Wasser gesetzt wurden, das Unrecht vergessen. Besonders der verschlossene Privatdetektiv Elia Contini, der zurückgezogen in einem Häuschen in den Bergen wohnt und am liebsten durch die Wälder streift, um Füchse zu fotografieren, denkt ungern an die Zeit zurück, in der sein Vater unter ungeklärten Umständen verschwand. Doch jetzt soll der Stausee erweitert und jener Teil des Sees trockengelegt werden, auf dem auch das Haus seiner Kindheit stand. Alte Wunden brechen auf. Als kurz hintereinander der Bürgermeister und ein Ingenieur ermordet werden, gerät Contini ins Fadenkreuz der Ermittler. Um sich selbst zu entlasten, muss er sich endlich der Vergangenheit stellen und herausfinden, was damals wirklich geschah ...</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>272 S.</t>
+          <t>978-3-7152-5503-3</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Atlantis Zürich</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>43216342</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>978-3-305-00492-8</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>«Jetzt kehre ich als Bettler dorthin zurück, wo man Vater um sein Erbe betrogen hat.» Am 18. Juli 1930 verlässt Hannes mit seiner Familie Georgien, das Land, in dem er geboren wurde. Simon, sein Vater, war 1866 in Langnau im Emmental aufgebrochen, um in Grusinien, wie die Russen Georgien nannten, seinen Traum zu verwirklichen: ein Geschlecht von angesehenen Bauern zu gründen. Als Simon 1918 starb, hinterliess er Hannes einen Gutshof mit mehr als tausend Kühen. Doch nach dem Einmarsch der Roten Armee und der Machtübernahme der Bolschewiki in Transkaukasien verliert die Familie ihren ganzen Besitz. Die Schweizer Auswanderer dürfen nicht mehr mitnehmen, als in einem Koffer Platz hat. Und sie haben noch Glück: Die deutschen Kolonisten werden deportiert - viele von ihnen verlieren in Sibirien ihr Leben. Der letzte Band von Werner Rysers kaukasischer Tetralogie hat beklemmende Parallelen zu aktuellen Ereignissen auf der Welt. Es scheint, als wiederhole sich die Geschichte. Immer wieder. «Kaukasische Sinfonie» ist der dritte Band einer Familiensaga, die mit den Romanen «Geh, wilder Knochenmann!» und «Die grusinische Braut» begonnen hat. Der Roman spielt vor dem Hintergrund weltgeschichtlicher Ereignisse: des Grossen Kriegs von 1914/18 und der Russischen Revolution, die das Schicksal der Menschen im kleinen Land zwischen dem Schwarzen und dem Kaspischen Meer prägen.</t>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 33 mmGewicht396 g</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>55771950</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Als lebten wir in einem barmherzigen Land </t>
+          <t>Die Schweiz und ihre Neutralität</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>49.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Kennedy, A. L. / Herzke, Ingo (Übers.) / Höbel, Susanne (Übers.)</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hanser C.</t>
-        </is>
-      </c>
+          <t>Jorio, Marco</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CHF 37.90</t>
+          <t>Die Schweiz sucht ihre Rolle in Europa und der Welt nicht erst seit dem Ausbruch des Kriegs in der Ukraine. Mit dem schrittweisen Aufbau der Europäischen Union und dem Ende des Kalten Krieges (1989) hat sich die internationale Lage unseres Landes von Grund auf geändert. Die Schweiz muss sich überlegen, welche Haltung sie als Staat mitten in Europa einnimmt und wie sie sich nach dem Untergang der bipolaren Welt positioniert. In diesen Diskussionen spielt die Neutralität eine zentrale Rolle. Aus der Staatsmaxime ist ein nationales Identitätsmerkmal geworden. Woher kommt diese tiefe Verankerung in der Bevölkerung? Wie konnte die Neutralität die Identität des Landes dermassen prägen? Wie, wann und warum entstand sie? Und können aus der Vergangenheit Perspektiven für die Zukunft aufgezeigt werden?Der Blick auf 400 Jahre Neutralitätsgeschichte gibt Antworten auf diese Fragen. 50 Jahre nach dem monumentalen Werk von Edgar Bonjour (1965-1970) legt der Historiker Marco Jorio eine neue Gesamtdarstellung zum Thema auf der Basis der Forschungen der letzten Jahrzehnte vor.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>464 S.</t>
+          <t>978-3-03919-389-9</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>hier + jetzt</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>42422100</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>978-3-446-27624-6</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>15.04.2023</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Ein Meisterwerk der moralischen Beunruhigung - die Weltpremiere von A.L. Kennedys neuem Roman. Soll man Unbarmherzigen gegenüber barmherzig sein? Anna unterrichtet an einer Grundschule und möchte immer noch die Welt verbessern. Wie vor fünfundzwanzig Jahren, als sie in Edinburgh mit einer Gruppe von Straßenkünstlern gegen die Kriegs- und Sozialpolitik der englischen Regierung demonstrierte. Was sie damals nicht ahnte: Einer ihrer Kumpane war ein V-Mann, der sie alle verriet. Nun stellt sie dem Peiniger nach. Doch bis wohin reicht das Böse - und kann Anna sich selber davon freihalten? Ein Meisterwerk der moralischen Beunruhigung. In ihrem unnachahmlichen Stil, in dem sich Ironie und Empathie verbinden, erzählt A.L. Kennedy von der Möglichkeit der Liebe der Menschen füreinander.</t>
-        </is>
-      </c>
+          <t>Breite 160 mm, Höhe 240 mm, Dicke 33 mmGewicht1134 gIllustrationenca. 20 sw und farbige Abbildungen</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Brüderchen </t>
+          <t>Der Campingplatzkiller</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Roman | Prix Goncourt des Lycéens und Prix Femina</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dupont-Monod, Clara / Finck, Sonja (Übers.)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Piper Hardcover</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CHF 30.50</t>
+          <t>Camping erfreut sich immer großerer Beliebtheit. Statt spießiger Kleinbürgeridylle ist das »Vanlife« auch in der jüngeren Generation angekommen: Ausgebuchte Platze, in der Hauptsaison sogar Wartelisten. Für die Dauercamper sind Touristen unerwünschte Eindringlinge in ihr Paradies. Heinrich »Henry« Kummer ist nicht ganz freiwillig auf dem Campingplatz gelandet. Mit 60 hat er seine Frühpensionierung beantragt - »So einen Bauchschuss lasst einen nachdenken«. Polizist war er, 32 Jahren lang. Aber keiner, der Verbrecher jagt, nicht einmal einer, der den Verkehr regelt. Als sich ihm die Gelegenheit geboten hat, ließ er sich in den Hausdienst versetzen. Und ist hangen geblieben. 25 Jahre hat er am Empfang des Kripo-Gebaudes in der Zürcher Kasernenstrasse verbracht. War für den Hausdienst zustandig, eine Art Abwart oder Portier. Und doch wurde ausgerechnet er bei einem Einsatz lebensgefahrlich verletzt. Aber auch das war keine Heldentat: Er war nur zur falschen Zeit am falschen Ort. Kummers neues Leben auf vier Radern beginnt weniger erholsam als gedacht: Dauercamperin Rosa wird tot in ihrem Wohnwagen gefunden: durchgeschnittene Kehle, ein einziger, sauberer Schnitt. Kummer ware nicht sein halbes Leben Polizist gewesen, wenn er den Ermittlungen tatenlos vom Campingstuhl aus zusehen würde ...</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>176 S.</t>
+          <t>978-3-7152-5506-4</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Atlantis Zürich</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>42388286</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>978-3-492-07175-8</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>»Poetisch, einfühlsam und zart: Eine wunderbare Ode an das Leben.« Le Figaro Magazine</t>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 25 mmGewicht270 g</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>55898510</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Die Wahrheit </t>
+          <t>Die Mitternachtsrose</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Roman - Nach den SPIEGEL-Bestsellern "Die Lüge" und "Die Bosheit" der neue packende Roman vom skandinavischen Meister der subtilen Spannung!</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Edvardsson, Mattias / Krummacher, Annika (Übers.)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Limes Verlag</t>
-        </is>
-      </c>
+          <t>Riley, LucindaHauser, SonjaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>CHF 23.90</t>
+          <t>Innerlich aufgelöst kommt die amerikanische Schauspielerin Rebecca Bradley im englischen Dartmoor an, wo ein altes Herrenhaus als Kulisse für einen Film dient, der in den 1920er Jahren spielt. Vor ihrer Abreise hat die Nachricht von Rebeccas angeblicher Verlobung eine Hetzjagd der Medien auf die junge Frau ausgelöst, doch in der Abgeschiedenheit von Astbury Hall kommt Rebecca allmählich zur Ruhe. Als sie jedoch erkennt, dass sie Lady Violet, der Großmutter des Hausherrn, frappierend ähnlich sieht, ist ihre Neugier geweckt. Dann taucht Ari Malik auf: ein junger Inder, den das Vermächtnis seiner Urgroßmutter Anahita nach Astbury Hall geführt hat. Und gemeinsam kommen sie nicht nur Anahitas Geschichte auf die Spur, sondern auch dem dunklen Geheimnis, das wie ein Fluch über der Dynastie der Astburys zu liegen scheint ...</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>448 S.</t>
+          <t>978-3-442-49429-3</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>42940283</t>
+          <t>20.04.2023</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>978-3-8090-2758-4</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>Deutsche Erstausgabe</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Ein Doppelmord, drei Verdächtige und nur eine Wahrheit - der neue, nervenzerreißend spannende Roman von SPIEGEL-Bestsellerautor Mattias Edvardsson.</t>
-        </is>
-      </c>
+          <t>Breite 128 mm, Höhe 188 mm, Dicke 39 mmGewicht440 g</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Der Morgen </t>
+          <t>Das kleine WIR in der 1. Klasse</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Thriller | Die neue Serie des Bestseller-Autors - dieses Buch bringt Sie um den Schlaf!</t>
+          <t>13.90</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Raabe, Marc</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Ullstein Extra</t>
-        </is>
-      </c>
+          <t>Herrenbrück, AnjaKunkel, Daniela</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>CHF 24.90</t>
+          <t>Schulanfang und das kleine WIR
+Auch die Kinder der ersten Klasse haben ein kleines WIR. Ob Matheunterricht, Lesen und Schreiben, Sport oder große Pause - mit dem WIR macht alles doppelt so viel Spaß. Doch die Schüler_innen der Wolkenklasse sind nicht immer einer Meinung. Sie haben auch mal Streit oder sagen blöde Sachen. Dann verschwindet das kleine WIR, und die Kinder vermissen es sehr. Denn ohne WIR-Gefühl fehlt der Wolkenklasse der Zusammenhalt. Zum Glück wissen die Schüler_innen, wie sie ihr WIR aufstöbern und aufpäppeln können. Bald ist ihr kleines WIR groß und stark. Und eins ist klar: Gemeinsam ist es einfach am schönsten!
+Unterstützt Kinder beim Lösen von KonfliktenEmpowert Kinder, füreinander da zu sein und gegen Ausgrenzung einzustehenAnschaulich und erstlesefreundlich erzähltGeeignet für Vor- und Grundschüler_innen
+Einfach Lesen lernen:
+1. Lesestufe: große Fibelschrift, leichte Wörter Kleine Texteinheiten in Kombination mit vielen bunten BildernComicelemente, um die Sehgewohnheiten von Kindern zu berücksichtigen
+lebensnahe Geschichte aus dem Kinderalltag
+Freundschaft, Zusammenhalt und WIR-Gefühl: ein wichtiges Thema, besonders für Erstlesekinder in der 1. Klasse. Das beliebte kleine WIR, jetzt auch zum ersten Lesen!</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>592 S.</t>
+          <t>978-3-551-69026-5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Carlsen</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>42576454</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>978-3-86493-205-2</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>Art Mayer-Serie</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Macht. Ohnmacht. Tatnacht.</t>
-        </is>
-      </c>
+          <t>Breite 160 mm, Höhe 215 mm, Dicke 15 mmGewicht286 gIllustrationenFarb. Abb.</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Biblioteca criminale </t>
+          <t>Idefix und die Unbeugsamen - Der Wecker von Lutetia - Erstlesebuch zur Serie</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pellegrinis vierter Fall</t>
+          <t>16.90</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Minardi, Dino</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Kampa Verlag</t>
-        </is>
-      </c>
+          <t>Uderzo, RenéGoscinny, AlbertJöken, KlausÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>CHF 23.90</t>
+          <t>In Lutetia stimmt etwas nicht. Alle Gallier haben verschlafen. Wo ist nur Sinfonix, der Hahn, dessen donnerndes Kikiriki sie normalerweise aus dem Schlaf reißt? Wurde er vielleicht von den Römern entführt? Idefix und seine Freunde müssen der Sache rasch auf den Grund gehen, bevor ihr Freund als Brathähnchen endet!Die Abenteuer von Idefix nacherzählt zum eingenständigen lesen, mit vielen Bildern aus der TV-Serie!</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>224 S.</t>
+          <t>978-3-7704-0731-6</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Ehapa Comic Collection</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>42907426</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>978-3-311-12058-2</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Ein Fall für Pellegrini</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>04</t>
-        </is>
-      </c>
+          <t>08.05.2023</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Die Tagung der Vereinigung Hominis et Tigris findet in diesem Jahr in der altehrwürdigen Bibliothek in der Città Alta von Bergamo statt. Kriminalistisch Interessierte aus ganz Europa kommen zusammen, unter ihnen auch Commissario Marco Pellegrini von der Polizia di Stato in Como. Doch noch vor dem ersten Vortrag wird klar, dass die Konferenz nicht wie ge­plant stattfinden kann. Der Archivar der Biblio­thek, Bertoldo Novarese, ein schmächtiger Mann mit Brille und grauen Locken, wurde mitten in der Nacht erschlagen. Ausgerechnet mit einem Folianten! Niemand hatte zu dieser Uhrzeit Zutritt zur Bibliothek - außer den Konferenzteilnehmenden, die im Lesesaal zu einer nächtlichen Gesprächsrunde zusammengekommen waren. Zwar wurde der Archivar von vielen für seine Pedanterie belächelt, aber ein Mordmotiv gibt das nicht her. Oder sind die Schätze, die Novarese hütete, kostbarer, als die meisten meinen? Pellegrini übernimmt den Fall und muss in den eigenen Reihen ermitteln. Auch privat kommt er nicht zur Ruhe: Franca ist ihm noch eine Antwort schuldig, und die wird sein ganzes Leben verändern.</t>
+          <t>Breite 153 mm, Höhe 216 mm, Dicke 10 mmGewicht304 g</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>55687597</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tochter einer leuchtenden Stadt </t>
+          <t>Trügerische Provence</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Roman | Vier Frauenschicksale, für immer miteinander verwoben durch die Liebe zur Heimat</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Suman, Defne / Meier, Gerhard (Übers.)</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>List</t>
-        </is>
-      </c>
+          <t>Lagrange, Pierre</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>CHF 32.90</t>
+          <t>Ein trügerischer Festspiel-Sommer in der Provence - der siebte Band der Provence-Krimi-Reihe von Bestseller-Autor Pierre Lagrange
+Mitten in der Konzertsaison in der Provence verschwinden plötzlich namhafte Musikerinnen. Die Ermittlungskommission unter Leitung von Caterine Castel und Alain Theroux tappt im Dunkeln. Es gibt keine Hinweise oder Forderungen im Zusammenhang mit der Entführung. Obwohl Ex-Commissaire Albin Leclerc mitten in den eigenen Hochzeitsvorbereitungen steckt, kann er es mal wieder nicht lassen: zusammen mit seinem Mops Tyson nimmt er die Spur auf. Als es zu einer weiteren Entführung kommt, und auch die kostbaren Instrumente verschwinden, stellt sich für ihn die Frage, ob in der Provence ein Wahnsinniger unterwegs ist. Die Ermittlungen bringen Albin Leclerc in allergrößte Gefahr ...</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>496 S.</t>
+          <t>978-3-596-70646-4</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Fester Einband</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>FISCHER Taschenbuch</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>42788362</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>978-3-471-36055-2</t>
-        </is>
-      </c>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.07</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Vom Untergang einer Stadt und einer Liebe, die alle Grenzen überwindet </t>
-        </is>
-      </c>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bretonische Idylle </t>
+          <t>Every (deutsche Ausgabe)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kommissar Dupins zehnter Fall</t>
+          <t>22.90</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bannalec, Jean-Luc</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
+          <t>Eggers, DaveTimmermann, KlausÜbersetzungWasel, UlrikeÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Der Circle ist die größte Suchmaschine gepaart mit dem größten Social-Media-Anbieter der Welt. Eine Fusion mit dem erfolgreichsten Onlineversandhaus brachte das reichste und gefährlichste - und seltsamerweise auch beliebteste - Monopol aller Zeiten hervor: Every.
+Delaney Wells ist »die Neue« bei Every und nicht gerade das, was man erwarten würde in einem Tech-Unternehmen. Als ehemalige Försterin und unerschütterliche Technikskeptikerin bahnt sie sich heimlich ihren Weg, mit nur einem Ziel vor Augen: die Firma von innen heraus zu zerschlagen. Zusammen mit ihrem Kollegen, dem nicht gerade ehrgeizigen Wes Kavakian, sucht sie nach den Schwachstellen von Every und hofft, die Menschheit von der allumfassenden Überwachung und der emojigesteuerten Infantilisierung zu befreien. Aber will die Menschheit überhaupt, wofür Delaney kämpft? Will die Menschheit wirklich frei sein?
+Wie schon bei »Der Circle« weiß Dave Eggers wie kein Zweiter unsere Wirklichkeit so konsequent weiterzudenken, dass einem der Atem stockt beim Lesen. Man kann nur inständig hoffen, dass die Realität nicht schneller voranschreitet, als Dave Eggers schreiben kann.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>978-3-462-00442-7</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>Kiepenheuer &amp; Witsch</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>CHF 18.50</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>336 S.</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>42779812</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>978-3-462-00489-2</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Kommissar Dupin ermittelt</t>
-        </is>
-      </c>
+          <t>04.05.2023</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Malerische Abgründe - Kommissar Dupin ermittelt auf der legendären Belle-Île.</t>
-        </is>
-      </c>
+          <t>Breite 126 mm, Höhe 191 mm, Dicke 25 mmGewicht374 g</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hohenrain </t>
+          <t>Pferdeflüsterer-Academy, Band 12: Wild und verwundbar</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kriminalroman</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Greiner, Patrick</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Emons</t>
-        </is>
-      </c>
+          <t>Mayer, Gina</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>CHF 19.90</t>
+          <t>Im wilden Kanada steht ein weißes Schloss: Snowfields. Auf dem Internat werden die weltbesten Reiter ausgebildet und verletzte Pferdeseelen geheilt.
+Zwei Neue in Snowfields sorgen für Liebeschaos pur. Der attraktive Schüler Petter, zu dem sich Zoes Freundin Isabelle stark hingezogen fühlt. Und die junge Lehrerin, die bei einigen Lehrkräften heftigste Gefühle auslöst. Doch auch auf anderer Ebene herrscht Chaos. Im Internet kursieren schlimme Gerüchte über den Pferdeflüsterer Caleb. Und so langsam beschleicht Zoe das Gefühl, dass das nicht alles nur Lügen sind ...
+Entdecke alle Abenteuer an der "Pferdeflüsterer-Academy":
+Band 1: Reise nach Snowfields
+Band 2: Ein geheimes Versprechen
+Band 3: Eine gefährliche Schönheit
+Band 4: Verletztes Vertrauen
+Band 5: Zerbrechliche Träume
+Band 6: Calypsos Fohlen
+Band 7: Flammendes Herz
+Band 8: Zoes größter Sieg
+Band 9: Cyprians Rückkehr
+Band 10: Die dunkle Wahrheit</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>320 S.</t>
+          <t>978-3-473-40461-2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>42832771</t>
+          <t>01.05.2023</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>978-3-7408-1686-5</t>
+          <t>1. Aufl.</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>HC - Pferdeflüsterer-Academy</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Malerische Abgründe - Kommissar Dupin ermittelt auf der legendären Belle-Île.</t>
-        </is>
-      </c>
+          <t>Breite 147 mm, Höhe 216 mm, Dicke 24 mm</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stumme Schreie </t>
+          <t>Twisted Games</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Flint &amp; Cavalli ermitteln hinter verschlossenen Türen. Kriminalroman. Ein Fall für Flint und Cavalli (9)</t>
+          <t>20.90</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ivanov, Petra</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Unionsverlag</t>
-        </is>
-      </c>
+          <t>Huang, AnaHallmann, MaikeÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>CHF 22.00</t>
+          <t>Sie ist eine Prinzessin. Er ihr Bodyguard. Ihr Beschützer. Ihr RuinGefangen von den Fesseln der Pflicht hat Bridget von Ascheberg, Prinzessin von Eldorra, nur drei Wünsche: Liebe, Leidenschaft und ihre eigenen Entscheidungen treffen zu dürfen. Doch als ihr Bruder seinen Anspruch auf den Thron aufgibt, findet sie sich auf einmal als zukünftige Königin wieder. Ein Titel, den sie nie wollte. An ihrer Seite der Mann, dem ihr Herz gehört, aber den sie nicht lieben darf: Rhys Larsen, ihr Bodyguard, ihr Beschützer, ihr Ruin. Ihre verbotenen Gefühle könnten sie beide in den Untergang treiben - und ihr Königreich zerstören.»Mitreißend, verboten und absolut süchtig machend - die Geschichte von Bridget und Rhys überzeugt mit einem perfekten Mix aus Gefühl, Leidenschaft und Tiefe.« CHARLEEN von CHARLIE_BOOKS Band 2 der heißen und romantischen TWISTED-Reihe von Bestseller-Autorin Ana Huang</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>352 S.</t>
+          <t>978-3-7363-1922-6</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>LYX</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>42890567</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>978-3-293-20952-7</t>
-        </is>
-      </c>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Ein Fall für Flint &amp; Cavalli; Unionsverlag Taschenbücher; metro</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.02</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Bruno Cavalli und Regina Flint stehen vor ganz neuen Herausforderungen. Cavalli kehrt nach langem Aufenthalt in den USA in die Schweiz zurück und tritt eine neue Stelle an. Dort wartet eine heikle Aufgabe auf ihn: Er soll einen Vorwurf gegen einen Polizisten untersuchen.</t>
-        </is>
-      </c>
+          <t>Breite 135 mm, Höhe 215 mm, Dicke 41 mm</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">SORRY. Ich habe es nur für dich getan </t>
+          <t>Fußball Academy 3: Eine große Überraschung</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Roman - ***Mit wunderschön farbig gestaltetem Buchschnitt nur in limitierter Auflage***</t>
+          <t>18.90</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Iosivoni, Bianca</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Penguin Verlag TB</t>
-        </is>
-      </c>
+          <t>Margil, IreneSchlüter, AndreasSaße, JanIllustrationen</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>CHF 21.50</t>
+          <t>Training, Team und Tore - diesmal zusammen mit einer Mädchen-Fußballmannschaft!
+Yao und seine Freunde erleben in der Academy jeden Tag Training, Toreschießen und Türenknallen. Immer ist was los. Eines Tages ist das Fußball-Internat plötzlich voller Mädchen. Ein neues Team von jungen Fußballerinnen aus ganz Europa beginnt die Elite-Ausbildung. Und sie sind starke Spielerinnen! Die Jungs sind verunsichert. Sollen sie gegen Mädchen spielen? Können Mädchen eine Mannschaft sein? Schnell lernen sie Amanda, Maike, Nayara und die anderen kennen und respektieren. Eine schöne gemeinsame Zeit beginnt.
+Über Unterschiede und Gemeinsamkeiten von Jungs und Mädchen im FußballZeigt, wie man als Mannschaft wächstFrauenfußball bleibt Fußball!</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>400 S.</t>
+          <t>978-3-551-65208-9</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Carlsen</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>42940246</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>978-3-328-10889-4</t>
-        </is>
-      </c>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Originalausgabe</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>n-Nr.03</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Die Erstauflage ist mit einem hochwertigen farbigen Buchschnitt ausgestattet - nur solange der Vorrat reicht.</t>
-        </is>
-      </c>
+          <t>Breite 148 mm, Höhe 220 mm, Dicke 25 mm</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Das Mädchen mit dem Drachen </t>
+          <t>Man vergisst nicht, wie man schwimmt</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Colombani, Laetitia / Marquardt, Claudia (Übers.)</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Fischer Taschenb.</t>
-        </is>
-      </c>
+          <t>Huber, Christian</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>»Die einzige Möglichkeit, etwas vom Leben zu haben, ist, sich hineinzuwerfen.«
+31. August 1999. Sengende Hitze liegt über Bodenstein, dem Heimatkaff des 15-jährigen Pascal. Es sind die großen Ferien, und eigentlich könnte der Junge den Sommer genießen. Den Skatepark. Die Partys der Oberstufler. Das Freibad mit den besten Pommes des Planeten. Doch seit er nicht mehr schwimmen kann, mag Pascal den Sommer nicht mehr. Warum das so ist, das kann er nicht erzählen. Ebenso wenig, wieso ihn alle Krüger nennen. Und erst recht nicht, warum er sich unter keinen Umständen verlieben darf. Lieber träumt er vor sich hin und schreibt Geschichten. Dann kracht Jacky in seine Welt. Ein geheimnisvolles Mädchen aus dem Zirkus. Mit roten Haaren, wasserblauen Augen und keiner Angst vor nichts. Zusammen verbringen sie einen flirrenden, letzten Sommertag, der alles für immer verändert ...</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>272 S.</t>
+          <t>978-3-423-21856-6</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>DTV</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>42780402</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>978-3-596-70678-5</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>»Das Mädchen mit dem Drachen« - nach »Der Zopf« und »Das Haus der Frauen« der neue Roman der Bestsellerautorin Laetitia Colombani</t>
-        </is>
-      </c>
+          <t>Breite 122 mm, Höhe 191 mm, Dicke 29 mmGewicht329 g</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dunkelwald </t>
+          <t>Five Survive</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kriminalroman</t>
+          <t>26.90</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mo, Johanna / Brauns, Ulrike (Übers.)</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Heyne Taschenb.</t>
-        </is>
-      </c>
+          <t>Jackson, HollyAgnew, Cherokee MoonÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>CHF 21.50</t>
+          <t>Eigentlich sollte es ein spaßiger Ausflug werden: Red ist mit fünf Freunden losgefahren, um Spring Break zu feiern. Doch unterwegs bleibt der alte Campingbus liegen - und sie stecken mitten im Nirgendwo fest. Kein Empfang, keine Aussicht auf Hilfe. Und es kommt noch schlimmer, denn draußen im Dunkeln lauert jemand. Sobald sie den Bus verlassen, schießt er auf sie. Seine Behauptung: Jemand aus der Gruppe verheimlicht etwas. Doch wen meint er? Alle sind gezwungen, ihre brisantesten Geheimnisse preiszugeben. Die Spannungen innerhalb des engen Campers steigen. Und nicht alle werden die Nacht überleben ...</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>496 S.</t>
+          <t>978-3-8466-0182-2</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Lübbe ONE in der Bastei Lübbe AG</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>35059579</t>
+          <t>28.04.2023</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>978-3-453-42582-8</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Deutsche Erstausgabe</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Die Hanna Duncker-Serie</t>
-        </is>
-      </c>
+          <t>1. Aufl. 2023</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Eine kleine Pension am See - ein Ort für das Glück</t>
-        </is>
-      </c>
+          <t>Breite 145 mm, Höhe 215 mm, Dicke 35 mmGewicht641 g</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Die Rebellin und der Dieb </t>
+          <t>Ein Lied über der Stadt</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Sendker, Jan-Philipp</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Heyne Taschenb.</t>
-        </is>
-      </c>
+          <t>Arenz, Ewald</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Sommer 1929 in einer Kleinstadt in Franken: Die Pfarrerstochter Luise träumt davon, das Fliegen zu erlernen. Gegen alle Widerstände gelingt es ihr, ihren Traum zu verwirklichen und Pilotin zu werden. Sie verlässt ihre Heimat und wird in München eine gefeierte Kunstpilotin. Als die Nazis an die Macht kommen, muss sie die Fliegerei aufgeben und kehrt nach Franken zurück. Hier ist plötzlich alles anders: Alle schweigen, ganz egal, was passiert. Angst und Misstrauen beherrschen das Miteinander. In der veränderten politischen Lage geraten Louises Familie und auch ihre Jugendliebe Georg mehr und mehr in Gefahr. Ihr Vater, der Terror und Verfolgung anprangert, wird denunziert und von der Gestapo bedroht und Georg als Mitglied des Widerstands gesucht. Schließlich werden Luises Liebe und ihr Können als Pilotin auf eine schwere Probe gestellt.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>320 S.</t>
+          <t>978-3-8321-6669-4</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>DuMont Buchverlag Gruppe</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>38616351</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>978-3-453-42706-8</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Erstmals im TB</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Die universelle Geschichte zweier Liebender aus verschiedenen Welten, die lernen, was im Angesicht einer Katastrophe zählt: Mut zum Widerstand, Wille zur Veränderung und bedingungsloses Vertrauen ineinander.</t>
-        </is>
-      </c>
+          <t>Breite 125 mm, Höhe 190 mm, Dicke 23 mmGewicht320 gIllustrationenUmschlag mit Strukturkarton, Hochprägung und Lack, Erstmals im Taschenbuch,</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Das Talent </t>
+          <t>Twisted Fate, Band 1: Wenn Magie erwacht (Epische Romantasy von SPIEGEL-Bestsellerautorin Bianca Iosivoni | Limitierte Auflage mit Farbschnitt)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>30.90</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Grisham, John / Walsh-Araya, Imke (Übers.)</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Heyne Taschenb.</t>
-        </is>
-      </c>
+          <t>Iosivoni, BiancaLiepins, CarolinUmschlaggestaltung</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>___ Limitierte Auflage mit farbigem Buchschnitt! Nur solange der Vorrat reicht! ___
+Als Faith ein Stipendium ergattert, hofft sie vor allem auf eins: ein ganz normales Studium. Doch als sie auf dem Campus auf ein Symbol mit gekreuzten Schwertern und Disteln stößt, ahnt sie, dass ihre Vergangenheit ihr gefolgt ist. Denn plötzlich steht Nate vor ihr, ein Freund aus Kindertagen mit dem gleichen Symbol als Tattoo auf der Haut. Aber auch Jax, der hemmungslos mit Faith flirtet, verbirgt etwas. Was Faith nicht ahnt: Ein längst vergessener Feind hat ihr gemeinsames Schicksal besiegelt.
+Weitere actiongeladene und herzzerreißende Romantasy von Bianca Iosivoni:
+Sturmtochter, Bd. 1-3
+Soul Mates, Bd. 1 &amp; 2
+The Last Goddess, Bd. 1 &amp; 2</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>416 S.</t>
+          <t>978-3-473-40219-9</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t>38615744</t>
+          <t>24.04.2023</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>978-3-453-44166-8</t>
+          <t>1. Aufl.</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Erstmals im TB</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>HC - Twisted Fate</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>"Beim Müll geht es ja immer um das Trennen. Darum sag ich, Müll beste Schule für das Denken. Weil du hast die Kategorien, sprich Wannen. Ohne die klare Trennung kannst du jedes Recycling vergessen. Und da bin ich noch nicht einmal bei den Problemstoffen."</t>
-        </is>
-      </c>
+          <t>Breite 154 mm, Höhe 217 mm, Dicke 41 mm</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nachtjagd </t>
+          <t>Eine Nacht, die vor 700 Jahren begann</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Thriller - Der Nr.1-Bestsellerautor aus Norwegen</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Fjell, Jan-Erik / Brunstermann, Andreas (Übers.)</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Goldmann</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>CHF 22.50</t>
+          <t>Während im Sommer 1944 deutsche Soldaten ungarische Dörfer plündern, stellen sich die Bauern in Kákásd immer noch dieselbe Frage wie vor 700 Jahren: Wie sollen sie leben von dem Lohn, den sie vom Grafen erhalten? Ein Streik könnte alles ändern. Doch in einer Zeit, in der ein Menschenleben billig und Weizen teuer ist, stehen die Chancen auf Erfolg schlecht. Ein junges Liebespaar auf der Flucht und ein Bauer bringen jedoch etwas ins Rollen, und das Leben im Dorf gerät aus den Fugen. Dieser Roman eines der größten ungarischen Romanciers war jahrzehntelang verschollen und erscheint hier zum allerersten Mal.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>512 S.</t>
+          <t>978-3-257-07236-5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>42939180</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>978-3-442-20648-3</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Deutsche Erstausgabe</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Vor einer Woche verschwand Lilli Sternberg.
-Ist sie die Tote am Strand von Sellnitz?
-Oder ist ein Serienmörder am Werk?</t>
-        </is>
-      </c>
+          <t>Breite 116 mm, Höhe 184 mm, Dicke 36 mmGewicht504 g</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Muschelträume </t>
+          <t>Gregs Tagebuch - Schulplaner 2023/2024</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>13.90</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Lassen, Svenja</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Blanvalet</t>
-        </is>
-      </c>
+          <t>Kinney, Jeff</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Der Schulplaner für alle Fans von Gregs Tagebuch! Volltreffer! Mit Gregs Schulplaner weißt du immer, wann der nächste Deutschtest ist, wann das Referat in Geschichte ansteht und wann das Training für deine Mannschaft stattfindet. So behältst du stets den Überblick über deine Termine, denn hier ist genug Platz für alle Aufgaben, Notizen und Verabredungen - für jeden Tag und jede Woche. So leicht war es noch nie, einen Plan zu haben - und auch noch nie so lustig!Hier drin findest du:_ Kalendarium von August 2023 bis August 2024_ Ferientermine 2023/2024_ Jahresübersicht 2023/2024_ Notentabelle_ Adressbuch für deine Freunde_ und viele witzige Comics aus den Greg-Büchern</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>368 S.</t>
+          <t>978-3-8339-0770-8</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Kalender</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Kalender</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Baumhaus Medien</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>42939800</t>
+          <t>28.04.2023</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>978-3-7341-1222-5</t>
+          <t>1. Aufl. 2023</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Originalausgabe</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Küstenliebe</t>
-        </is>
-      </c>
+          <t>Gregs Tagebuch</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr">
         <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="O26" t="inlineStr"/>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Breite 105 mm, Höhe 160 mm, Dicke 13 mm</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stranded - Die Insel </t>
+          <t>Mein Schülerkalender für Potterheads! 2023/2024</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Acht Fremde. Ein Mörder. Kein Ausweg. Thriller</t>
+          <t>21.50</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Goodwin, Sarah / Hanowell, Dr. Holger (Übers.)</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Bastei Lübbe TB</t>
-        </is>
-      </c>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>CHF 18.50</t>
+          <t>Magischer Schulalltag garantiert!
+Wo könnte man das neue Schuljahr besser beginnen als an der Schule für Hexerei und Zauberei? Mit dem neuen, magischen Schülerkalender für Potterheads bist du für den Schulalltag bestens gewappnet! Hier findest du alles, was du für die Organisation von Klausurenterminen, Hausaufgaben und Projekten benötigst:
+Praktische Wochen- und Monatsübersichten und Listen erleichtern die OrganisationSpannende Tests, zauberhafte Hacks und leckere Rezepte aus der Schule für Hexerei und ZaubereiMagische Gestaltung und hochwertige Ausstattung mit Glanzfolie und Leseband
+Finde heraus in welches Haus du gehörst, welches Haustier in Hogwarts am besten zu dir passt und teste dein Wissen über die Welt der Hexen und Zauberer! Dank magischen Illustrationen und der hochwertigen Ausstattung mit Leseband und Goldfolie ist er auch optisch ein echter Hingucker!</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>400 S.</t>
+          <t>978-3-7459-1568-6</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Edition Michael Fischer</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>38723826</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>978-3-404-18878-9</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>1. Aufl. 2023</t>
-        </is>
-      </c>
+          <t>19.04.2023</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr"/>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Breite 153 mm, Höhe 216 mm, Dicke 20 mmGewicht510 g</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sommerschwestern </t>
+          <t>Liar - Tödlicher Verrat</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Roman | Der SPIEGEL-Bestseller #1 von der Autorin der »Dienstagsfrauen«</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Peetz, Monika</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Kiepenheuer &amp; Witsch</t>
-        </is>
-      </c>
+          <t>Jackson, LisaLake-Zapp, KristinaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Eine skandalumwitterte Familie, eine verhängnisvolle Affäre und ein mörderischer Plan:
+Bestseller-Autorin Lisa Jackson begeistert mit einem dramatischen Thriller voller unvorhersehbarer Wendungen.
+Nach einem bösen Streit mit ihrem schwerreichen, notorisch untreuen Freund James Cahill will Megan Travers nur noch weg von dessen Ranch in den Cascade Mountains. Trotz eines heftigen Schneesturms macht sie sich auf den Weg zu ihrer Schwester, doch dort kommt sie nie an. Als die Detectives Brett Rivers und Wynonna Mendoza James befragen wollen, finden sie ihn mit einer Kopfverletzung im Krankenhaus vor. James sagt aus, er könne sich an nichts erinnern, weder an Megan noch an seine zahlreichen Affären. Kurz darauf bringen die Morde an zwei Frauen aus seinem Umfeld den Herzensbrecher in Erklärungsnöte ...
+Hochspannung, eine Prise Romantik, jede Menge zwischenmenschliche Verwicklungen und kaltblütige Morde - all das bietet dieser Thriller von Bestseller-Autorin Lisa Jackson. Liar - Tödlicher Verrat ist unabhängig lesbar.
+Entdecken Sie auch die anderen Thriller von Lisa Jackson, z.B. Showdown - Ich bin dein Tod um zwei Schwestern, die erbitterte Rivalinnen sind, oder Paranoid, worin es um späte Rache in einer ehemaligen Highschool-Clique geht.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>304 S.</t>
+          <t>978-3-426-52652-1</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Droemer/Knaur</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>42780273</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>978-3-462-00447-2</t>
-        </is>
-      </c>
+          <t>02.05.2023</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr">
         <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>Die Sommerschwestern-Romane</t>
-        </is>
-      </c>
+          <t>Ein San-Francisco-Thriller</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vier erwachsene Schwestern, die unterschiedlicher nicht sein könnten, folgen der rätselhaften Einladung ihrer kapriziösen Mutter zu einem Familientreffen am Ferienort ihrer Kindheit. Mit gemischten Gefühlen treffen sie im malerischen Örtchen Bergen an der holländischen Küste ein. Jede mit ihren eigenen Sorgen und Gedanken im Gepäck. Warum ruft die Mutter sie zusammen? </t>
-        </is>
-      </c>
+          <t>Breite 125 mm, Höhe 190 mm, Dicke 34 mm</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Gegen alle Regeln </t>
+          <t>Strandhaus Meeresrauschen</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Thriller</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cavanagh, Steve / Kinzel, Fred (Übers.)</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Goldmann</t>
-        </is>
-      </c>
+          <t>Säfstrand, CarolineWerner, StefanieÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Der Klang der Wellen, der Geruch des Meeres und ein Haus voller Bücher - der neue Roman von Schwedens Feel-Good-Königin Caroline Säfstrand!
+Die Autorin Inez lebt zurückgezogen in einem kleinen Strandhaus an der schwedischen Küste, sie umgibt sich lieber mit Büchern als mit Menschen. Als ihre Nachbarin stirbt, beschließt sie, mit ihrem Leben aufzuräumen: Sie möchte vorsorgen, ihr Haus ausmisten und ihr letztes, alles offenbarendes Buch schreiben. Als Inez kurz darauf stürzt, ist sie gezwungen, das Dienstmädchen Meja einzustellen. Sie soll ihr beim Entrümpeln des Strandhauses helfen. Die einzige Regel: Unter keinen Umständen darf der blaue Ordner mit dem Buchskript geöffnet werden! Doch natürlich sieht Meja die geheimen Worte eines Tages ... Das Treffen zwischen Inez, die im hohen Alter mit ihrer Vergangenheit versöhnt werden muss, und der hoffnungslosen Meja, die nach einer Zukunft sucht, hat für die beiden ungleichen Frauen unvorhergesehene Folgen ...
+Lust auf noch mehr schwedische Wohlfühllektüre? Dann lesen Sie auch »Strandhotel Meeresbrise« von Caroline Säfstrand.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>576 S.</t>
+          <t>978-3-7341-1241-6</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>38870114</t>
+          <t>20.04.2023</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>978-3-442-49406-4</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Eddie-Flynn-Reihe</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Als David Child wegen Mordes verhaftet wird, wendet sich das FBI an Strafverteidiger Eddie Flynn: Er soll Child vertreten und dazu bringen, als Zeuge gegen eine skrupellose Anwaltskanzlei auszusagen, die im Verdacht steht, an einem globalen Betrug beteiligt zu sein. Eddie bleibt keine Wahl, denn das FBI erpresst ihn mit belastenden Unterlagen über seine Ehefrau Christine, die ihre Unterschrift ahnungslos unter ein brisantes Dokument gesetzt hatte. Als er Child zum ersten Mal trifft, weiß er, dass der Mann unschuldig ist, auch wenn die Beweise gegen ihn überwältigend scheinen. Er muss einen Weg finden, Childs Unschuld zu beweisen und gleichzeitig seine Frau zu schützen - nicht nur vor dem FBI, sondern auch vor der Firma.</t>
-        </is>
-      </c>
+          <t>Breite 119 mm, Höhe 188 mm, Dicke 34 mmGewicht353 g</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Das Glück in den Wäldern </t>
+          <t>Good Places for Good People</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Ein Sehnsuchtswald-Roman</t>
+          <t>35.90</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Koelle, Patricia</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Fischer Taschenb.</t>
-        </is>
-      </c>
+          <t>Diallo, FranziskaHehl, Judith</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CHF 16.90</t>
+          <t>Dorthin reisen, wo Nachhaltigkeit gelebt wird
+Nachhaltigkeit wird inzwischen genauso selbstverständlich erwartet wie einmalige Erlebnisse und Erholung. Der Inspirations-Bildband Good Places for Good People präsentiert 50 Unterkünfte und Destinationen in Europa, die den aktuellen Umweltstandards nicht nur gerecht werden, sondern auch in jeder Preiskategorie für eine genuss- und stilvolle Auszeit sorgen.
+Ob Stadthotel oder Baumhaus, Wellness-Resort oder Bauernhof: Die Gastgeber:innen dieser handverlesenen Orte setzen sich für einen schonenden Umgang mit Ressourcen ein, kochen frisch und regional und engagieren sich für Natur und Menschen in ihrer Region. Die perfekte Inspiration für alle, die umweltbewusst reisen wollen - ohne Kompromisse.
+Wirklich nachhaltige Reiseideen für ein gutes Urlaubsgefühl</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>496 S.</t>
+          <t>978-3-95889-449-5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>42091910</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>978-3-596-70723-2</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>1. Auflage</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Sehnsuchtswald-Reihe</t>
-        </is>
-      </c>
+          <t>08.05.2023</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Manchmal führt der Weg zum Glück durch einen geheimnisvollen Wald - der zweite Band der Sehnsuchtswald-Reihe von Bestseller-Autorin Patricia Koelle </t>
-        </is>
-      </c>
+          <t>Breite 170 mm, Höhe 240 mm, Dicke 20 mmGewicht734 g</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hotel Freiheit </t>
+          <t>Alle Mamas</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sylt-Saga 3 - Roman</t>
+          <t>23.90</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pauly, Gisa</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Heyne Taschenb.</t>
-        </is>
-      </c>
+          <t>Ellis, Sarah KateEllis-Henderson, KristenRambaldi, MaxIllustrationenFiedler-Tresp, SonjaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CHF 21.50</t>
+          <t>»Alle Mamas« ist Liebesbrief und Lobeshymne an alle Mütter in einem. Die Botschaft ist: Alle Mütter zu feiern, weil sie unglaubliches leisten. Ob Pilotin, Ärztin, alleinerziehend, in Form zweier Väter oder als tolle Oma - alle Mütter zeichnen sich vor allem durch ihre Fürsorge und Liebe für ihre Kinder aus. Die zeitgemäßen, farbenfrohen Illustrationen stecken voller Leben und zeigen wie vielseitig Familien heute sind.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>432 S.</t>
+          <t>978-3-96846-113-7</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Deutsch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Kartonierter Einband (Kt)</t>
+          <t>GebundenFormatBilderbuch</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>Migo</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>36066149</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>978-3-453-42579-8</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Originalausgabe</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>Die Sylt-Saga</t>
-        </is>
-      </c>
+          <t>14.04.2023</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>Deutsch</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Brit, Kari und Alisia: drei Frauen und ihre Lebensträume - der dritte Band der großen Syltsaga
-Sylt, Gegenwart. Das berühmte Café und Hotel König Augustin wird mittlerweile von Kari geleitet, Brit hat sich aus dem Alltagsgeschäft zurückgezogen. Aber wie soll es weitergehen? Karis Tochter Alisia, die das Geschäft übernehmen soll, hat eine eigene Karriere: Sie ist ein gefragtes Model und erobert unter dem Namen "La Cappuccina" sämtliche Laufstege. Dann aber ändert sich alles, denn ihr begegnet die große Liebe. Dieser Mann scheint jedoch genau der Falsche zu sein...</t>
-        </is>
-      </c>
+          <t>Breite 224 mm, Höhe 287 mm, Dicke 9 mmGewicht368 g</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Star Switch â Mein (Dein) Leben steht Kopf</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Dixon, AleshaBirchall, KatyKilchling, VerenaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Ich bin du, und du bist ich
+Naomi ist dreizehn und der größte Popstar der Welt. Sie tritt in Amerika auf, tourt durch Japan, und alle, einfach alle finden sie toll. Aber richtige Freunde hat sie keine, und wenn sie mal shoppen gehen will, wird das Einkaufszentrum nur für sie geöffnet - nachts, wenn sonst niemand dort ist. Ruby ist Naomis größter Fan. Sie kennt die Texte zu jedem ihrer Lieder, sie kann alle Moves nachmachen und träumt heimlich davon, Naomis allerbeste Freundin zu sein. Als die beiden Mädchen zufällig aufeinandertreffen und - zack! - die Körper tauschen, gerät Ruby von einer Sekunde auf die nächste ins Rampenlicht. Wird sie ihr neues Superstar-Leben lieben oder wird sie am Ende genauso einsam sein wie Naomi? Und wird Naomi herausfinden, dass sie weltberühmt und doch ein normales Mädchen sein kann?
+Erfolgreiches Dream-Team: Die Bestsellerautorin Katy Birchall (»Emma Charming«) und der Show-Star Alesha Dixon (»Britan's Got Talent«) schreiben zusammen eine Körpertauschgeschichte voller Drehungen und Wendungen, bei der man nie weiß, was als Nächstes kommt - witzig, turbulent und charmant!</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>978-3-7373-4270-4</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>FISCHER KJB</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Breite 148 mm, Höhe 219 mm, Dicke 29 mmGewicht481 g</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Die Robot-Kids 1: Rettung von Moto-5</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>13.90</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Flessner, BerndFlessner, HannahGrubing, TimoIllustrationen</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Modernes Erstlesebuch mit den Robot-Kids
+In den Ferien besuchen Alex, Milo, Lea und deren Schwester Sam ein Forschungsinstitut. Alex' Tante Jana ist Roboter-Expertin und sie testet und entwickelt dort verschiedene Modelle. Die Kinder sind sofort Feuer und Flamme, als sie dort den ausrangierten Serviceroboter Moto-5 entdecken. Mit viel Köpfchen und Kreativität machen sie sich ans Werk. Denn wenn sie es schaffen, den Roboter wieder zum Laufen zu bringen, dürfen sie Moto-5 behalten!
+Ein spannendes Erstlese-Abenteuer, das Lust aufs Lesen macht.
+Kurze Kapitel, eingängiger Text, coole Illustrationen sowie eine Lese-Urkunde zur Belohnung motivieren zum Weiterlesen.
+Der Auftakt zur neuen Reihe "Die Robot-Kids" vom Bestseller-Duo Bernd und Hannah Flessner, mit tollen Bildern von Timo Grubing!
+Mit viel Witz, coolen Illustrationen und Leseurkunde gelingt es dem Autorenduo Flessner, ein wichtiges Zukunfsthema kindgerecht und spannend aufzuarbeiten.
+Am Ende erklärt der Roboter "Moto-5" in einem kleinen Wörterbuch die Fachbegriffe zusätzlich.
+------------------------------
+Die Robot-Kids, das sind: Alex, Milo, Lea und deren kleine Schwester Sam. Alex' Tante Jana ist Roboter-Expertin und häufig dürfen die Kinder sie in ihrem Forschungslabor besuchen. Dort gibt es viele unterschiedliche Roboter zu sehen, die verschiedenene Aufgaben zu erfüllen haben. Fast alle dienen dazu. Menschen in Situationen zu helfen und oft auch ihr Leben zu schützen, wie zum Beispiel die wie große Käfer aussehenden Löschroboter.
+Die Kinder dürfen auch beim Testen der Roboter zuschauen, und dabei geschehen immer wieder unvorhergesehene Dinge, die lustig, aber auch gefährlich sein können.
+Für viel Spaß sorgt auch Janas Mann Markus, der Erfinder ist und ebenfalls mit Robotern experimentiert. Seine Arbeit an einer Nudelmaschine ist auf jeden Fall noch verbesserungswürdig ...
+------------------------------
+In Band 1 "Rettung von Moto-5" (ISBN 978-3551690203) reparieren die Kinder den Service-Roboter Moto-5 und bewahren ihn so vor dem Verschrotten.
+In Band 2 "Die Löschroboter" (ISBN 978-3551690210, erscheint im Juli 2023) testen die Kinder Löschroboter bei einem vorgetäuschten Waldbrand und kommen dabei ganz schön ins Schwitzen.
+In Band 3 (erscheint im Juli 2024) werden die Kinder Robot-Kids ein Abenteuer in den Bergen erleben.
+Und alle, die weitere Abenteuer mit den Robot-Kids erleben wollen, dürfen sich freuen, denn es sind auch Abenteuer für fortgeschrittene Leser_innen geplant!
+------------------------------
+Einfach Lesen lernen:
+2. Lesestufe: Kurze Sätze, große SchriftKleine Texteinheiten in Kombination mit vielen bunten BildernComicelemente, um die Sehgewohnheiten von Kindern zu berücksichtigen
+Spannung, Abenteuer, Technik - packender Mix für Leseanfänger_innen ab 6Mit Lese-Urkunde und kleinem Wörterbuch zu Fachbegriffen</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>978-3-551-69020-3</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Carlsen</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>n-Nr.01</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Breite 160 mm, Höhe 215 mm, Dicke 12 mm</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Warum wir nicht durch Wände gehen*</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>36.90</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Aigner, Florian</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Die Welt der Quanten ist voller atemberaubender Geschichten und Ideen - von winzigen Teilchen, die sich an zwei verschiedenen Orten gleichzeitig befinden, von Katzen, die gleichzeitig lebendig und tot sind, von geheimnisvoller Teleportation. Gleichzeitig bestimmt Quantenphysik längst unseren Alltag: Laser, Mikrochips oder MRT-Bilder wären ohne Quantentheorie nicht möglich. Immer wieder heißt es: Quanten sind so kompliziert, dass sie höchstens von ein paar Wissenschaftsgenies verstanden werden können. Stimmt nicht, beweist Wissenschaftserklärer und Quantenphysiker Florian Aigner in seinem neuen Buch! Die Welt der Quanten kann jeder verstehen, wenn wir aus unseren gewohnten Denkmustern ausbrechen. Wie das gelingt, zeigt der Bestsellerautor auf einem Trip in die erstaunliche Welt der kleinsten Teilchen - unterhaltsam, höchst erhellend und horizonterweiternd.</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>978-3-7106-0689-2</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Brandstätter</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>24.04.2023</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Breite 142 mm, Höhe 218 mm, Dicke 27 mmGewicht558 g</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Peppino</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>24.90</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Ziegler, UrsinaJucker, SitaIllustrationen</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Peppinos Vater Peppone ist Schausteller. Als dieser sich verletzt, ist Peppino plötzlich auf sich allein gestellt. Er meistert diese Herausforderung bravourös, denn wie sich herausstellt, steckt im kleinen Peppino ein großer Künstler, der die Menschen mit seinen Bildern begeistert. » Peppino « erzählt die zeitlose Geschichte eines Jungen, der sich in schwierigsten Umständen behauptet. Das Buch erschien erstmals 1971 und transportiert den Geist seiner Zeit. Jetzt geben wir den Schweizer Bilderbuch-Klassiker in einer sorgfältig gestalteten Ausgabe neu heraus.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>978-3-314-10640-8</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Breite 280 mm, Höhe 215 mm, Dicke 15 mmGewicht402 gIllustrationenDurchgehend farbig illustriert</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Unkaputtbar: Mein erstes Wimmelbuch: Wir machen einen Ausflug</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>8.90</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Schumann, SibylleReckers, SandraIllustrationen</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Die unkaputtbaren Wimmelbücher, die alles mitmachen
+Komm, wir machen einen Ausflug: Was können wir im Wald alles entdecken? Wen triffst du im Tierpark? Und wo hat sich eigentlich der kleine Teddy versteckt? Ein erstes Wimmelbuch zum Suchen, Finden und Weitererzählen.
+Für alle Baby-Pixi-Fans: Die neue Wimmelbuchreihe kombiniert spannende Themen mit dem beliebten unkaputtbaren Material. Genau so leicht, handlich und robust wie die bekannten Baby Pixis - aber größer, umfangreicher und ideal für Kinder ab 2 Jahren. Die unkaputtbaren Wimmelbücher, die alles mitmachen!</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>978-3-551-06254-3</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Carlsen</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Unkaputtbar</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Breite 145 mm, Höhe 170 mm, Dicke 4 mmGewicht30 g</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new method to scrape all books
</commit_message>
<xml_diff>
--- a/data/excelfiles/df_neuheiten_blatter.xlsx
+++ b/data/excelfiles/df_neuheiten_blatter.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,21 +518,163 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Atlas - Die Geschichte von Pa Salt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>32.00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Riley, LucindaWhittaker, HarryHauser, SonjaÜbersetzungDufner, KarinÜbersetzungSchmidt, SibylleÜbersetzungWulfekamp, UrsulaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Paris, 1928. Ein Junge wird gerade noch rechtzeitig entdeckt, bevor er stirbt, und von einer Familie aufgenommen. Er ist klug und liebenswert, und er entfaltet seine Talente in dem neuen Zuhause. Hier wird ihm ein Leben ermöglicht, von dem er nicht zu träumen gewagt hätte. Doch er weigert sich, einen Hinweis darauf zu geben, wer er wirklich ist. Als er zu einem jungen Mann heranwächst, verliebt er sich und besucht das berühmte Pariser Konservatorium. Die Schrecken seiner Vergangenheit kann er darüber beinahe vergessen, ebenso wie das Versprechen, das er einst geschworen hat, einzulösen. Aber Unheil ballt sich zusammen über Europa, und niemand ist mehr in Sicherheit. Tief in seinem Herzen weiß er, dass die Zeit kommen wird und er wieder fliehen muss.
+Ägäis, 2008. Alle sieben Schwestern sind an Bord der »Titan« zusammengekommen, um sich von ihrem geliebten Vater, der ihnen stets ein Rätsel blieb, zu verabschieden. Zur Überraschung aller ist es die verschwundene Schwester, die von Pa Salt damit betraut wurde, ihnen die Spur in ihre Vergangenheit aufzuzeigen. Aber für jede Wahrheit, die enthüllt wird, taucht eine neue Frage auf, und die Schwestern müssen erkennen, dass sie ihren Vater kaum gekannt haben. Noch schockierender aber ist, dass diese lang begrabenen Geheimnisse noch immer Auswirkungen auf ihrer aller Leben haben.
+»Atlas. Die Geschichte von Pa Salt« erzählt von einem Leben voller Liebe und Verluste, umspannt Meere und Kontinente und führt die »Sieben-Schwestern«-Serie zu einer Atem beraubenden Auflösung.
+Harry Whittaker ist Lucinda Rileys Sohn, dem sie vor ihrem Tod die Geschichte von »Atlas« in die Hände gelegt hat, damit er sie nach ihren Vorstellungen zum Abschluss bringt.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>978-3-442-31567-3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Goldmann</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>11.05.2023Erstverkaufstag11.05.2023</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>n-Nr.08</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Atlas - Die Geschichte von Pa Salt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>32.00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Riley, LucindaWhittaker, HarryHauser, SonjaÜbersetzungDufner, KarinÜbersetzungSchmidt, SibylleÜbersetzungWulfekamp, UrsulaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Paris, 1928. Ein Junge wird gerade noch rechtzeitig entdeckt, bevor er stirbt, und von einer Familie aufgenommen. Er ist klug und liebenswert, und er entfaltet seine Talente in dem neuen Zuhause. Hier wird ihm ein Leben ermöglicht, von dem er nicht zu träumen gewagt hätte. Doch er weigert sich, einen Hinweis darauf zu geben, wer er wirklich ist. Als er zu einem jungen Mann heranwächst, verliebt er sich und besucht das berühmte Pariser Konservatorium. Die Schrecken seiner Vergangenheit kann er darüber beinahe vergessen, ebenso wie das Versprechen, das er einst geschworen hat, einzulösen. Aber Unheil ballt sich zusammen über Europa, und niemand ist mehr in Sicherheit. Tief in seinem Herzen weiß er, dass die Zeit kommen wird und er wieder fliehen muss.
+Ägäis, 2008. Alle sieben Schwestern sind an Bord der »Titan« zusammengekommen, um sich von ihrem geliebten Vater, der ihnen stets ein Rätsel blieb, zu verabschieden. Zur Überraschung aller ist es die verschwundene Schwester, die von Pa Salt damit betraut wurde, ihnen die Spur in ihre Vergangenheit aufzuzeigen. Aber für jede Wahrheit, die enthüllt wird, taucht eine neue Frage auf, und die Schwestern müssen erkennen, dass sie ihren Vater kaum gekannt haben. Noch schockierender aber ist, dass diese lang begrabenen Geheimnisse noch immer Auswirkungen auf ihrer aller Leben haben.
+»Atlas. Die Geschichte von Pa Salt« erzählt von einem Leben voller Liebe und Verluste, umspannt Meere und Kontinente und führt die »Sieben-Schwestern«-Serie zu einer Atem beraubenden Auflösung.
+Harry Whittaker ist Lucinda Rileys Sohn, dem sie vor ihrem Tod die Geschichte von »Atlas« in die Hände gelegt hat, damit er sie nach ihren Vorstellungen zum Abschluss bringt.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>978-3-442-31567-3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Goldmann</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>11.05.2023Erstverkaufstag11.05.2023</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>n-Nr.08</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Der Feind</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>24.90</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Brand, Christine</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Ein bizarre Mordserie an Männern sowie Schüsse während einer Frauendisko - in Band 5 der Erfolgsserie halten gleich zwei Fälle Milla Nova und das Team um Sandro Bandini auf Trab.
 Ein bizarrer Mord sorgt für Aufsehen: Ein Mann wurde an sein Bett gefesselt und hingerichtet. An den Füßen trägt er rote Stöckelschuhe. Schnell stellt sich heraus, dass er zuvor eine Drohung erhielt: ein Foto von sich selbst - mit dem Absatz eines Stöckelschuhs im Gesicht. Er ist nicht der Einzige, der solch eine Nachricht bekam. Sind auch die anderen Bedrohten in Gefahr? Gleichzeitig jagt das Team um Polizeichef Sandro Bandini einen Mann, der in einer Frauendisko in einem linken Kulturzentrum um sich schoss. Die Vermutung eines rechtsextremen Hintergrunds liegt nahe, doch TV-Reporterin Milla Nova vermutet ein anderes Motiv: Frauenhass. Gemeinsam mit ihrem blinden Freund Nathaniel taucht sie in die dunkle Welt der Incels ein. Zwei Fälle, bei denen der Hass auf das andere Geschlecht eine vitale Rolle spielt. Ist es Zufall oder besteht ein Zusammenhang?
@@ -545,306 +687,181 @@
 Lesen Sie auch »Wahre Verbrechen»: Christine Brand schreibt über ihre dramatischsten Fälle als Gerichtsreporterin.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>978-3-7645-0771-8</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Buch</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Paperback</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Blanvalet</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>26.04.2023</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>1. A.</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>n-Nr.05</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Der Feind</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>24.90</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Brand, Christine</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Ein bizarre Mordserie an Männern sowie Schüsse während einer Frauendisko - in Band 5 der Erfolgsserie halten gleich zwei Fälle Milla Nova und das Team um Sandro Bandini auf Trab.
+Ein bizarrer Mord sorgt für Aufsehen: Ein Mann wurde an sein Bett gefesselt und hingerichtet. An den Füßen trägt er rote Stöckelschuhe. Schnell stellt sich heraus, dass er zuvor eine Drohung erhielt: ein Foto von sich selbst - mit dem Absatz eines Stöckelschuhs im Gesicht. Er ist nicht der Einzige, der solch eine Nachricht bekam. Sind auch die anderen Bedrohten in Gefahr? Gleichzeitig jagt das Team um Polizeichef Sandro Bandini einen Mann, der in einer Frauendisko in einem linken Kulturzentrum um sich schoss. Die Vermutung eines rechtsextremen Hintergrunds liegt nahe, doch TV-Reporterin Milla Nova vermutet ein anderes Motiv: Frauenhass. Gemeinsam mit ihrem blinden Freund Nathaniel taucht sie in die dunkle Welt der Incels ein. Zwei Fälle, bei denen der Hass auf das andere Geschlecht eine vitale Rolle spielt. Ist es Zufall oder besteht ein Zusammenhang?
+Die unabhängig voneinander lesbaren Krimis um Milla Nova und Sandro Bandini:
+1. Blind
+2. Die Patientin
+3. Der Bruder
+4. Der Unbekannte
+5. Der Feind
+Lesen Sie auch »Wahre Verbrechen»: Christine Brand schreibt über ihre dramatischsten Fälle als Gerichtsreporterin.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>978-3-7645-0771-8</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Blanvalet</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>n-Nr.05</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Die Krume Brot</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>29.00</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>belletristik schweizer</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Adelina, Tochter italienischer Einwanderer, arbeitet in einer Zürcher Fabrik, als sie nach kurzem Liebesglück mit einem Kind allein dasteht. Sie verliert die Stelle, die Wohnung, kämpft ums Überleben. In der größten Not lernt sie Emil kennen, einen erfolgreichen Grafiker, der ihre Schulden bezahlt und Adelina mit der kleinen Emma bei sich aufnimmt. Außer an der Liebe fehlt es an nichts. Emil kauft ein Anwesen in den Bergen des Piemont und scheint auf gemeinsames Glück zu hoffen. Aber dann verschwindet das Kind, spurlos.
 Adelina macht sich auf die Suche, begleitet von einem schweigsamen Unbekannten. Er bringt sie nach Mailand, in eine Kommune, zu Menschen, die an die Revolution glauben und Adelina versprechen, die verlorene Tochter zu finden; sie muss nur bereit sein, sich dem Kampf anzuschließen, und mit ihren Schweizer Papieren über die Grenze gehen, auf eine gefährliche Mission.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>978-3-498-00320-3</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Buch</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Gebunden</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Rowohlt</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>18.04.2023</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Breite 133 mm, Höhe 209 mm, Dicke 23 mmGewicht330 g</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Der Magier im Kreml</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>36.90</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Da Empoli, GiulianoMeßner, MichaelaÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>SPIEGEL-BESTSELLER UND VIELFACH AUSGEZEICHNET
-Man nennt ihn den «Magier im Kreml». Der rätselhafte Vadim Baranow war Regisseur und Produzent von Reality-TV-Shows, bevor er zur grauen Eminenz von Putin wird. Nachdem er als politischer Berater von der Bühne verschwindet, werden immer mehr Legenden über ihn verbreitet. Bis er eines Nachts dem Ich-Erzähler dieses Buches, der seit Langem in Moskauer Archiven forscht, seine Geschichte anvertraut â¦
-Dieser Roman führt uns ins Zentrum der russischen Macht, wo permanent Intrigen gesponnen werden. Und wo Vadim, der zum wichtigsten Spindoktor des Regimes geworden ist, ein ganzes Land in ein politisches Theater verwandelt, in dem es keine andere Realität als die Erfüllung der Wünsche des Präsidenten gibt. Doch Vadim ist kein gewöhnlicher Ehrgeizling: Der Regisseur, der sich unter die Wölfe verirrt hat, gerät immer tiefer in die Machenschaften des Systems, das er selbst mit aufgebaut hat, und wird alles daransetzen, um dort wieder herauszukommen. Er nimmt den Erzähler mit auf eine Reise ins Herz der Finsternis. «Der Magier im Kreml» ist ein großer Roman über das zeitgenössische Russland und die Entstehung seiner medial inszenierten und vollkommen fiktiven, aber auch tödlichen Realität, einem Imperium der Lüge. Er enthüllt nicht nur die Hintergründe der Putin-Ära, sondern bietet auch eine hellsichtige Betrachtung über die Macht.
-Ausgezeichnet mit dem Grand Prix du Roman de l Académie française
-Finalist des Prix Goncourt 2022
-200 000 verkaufte Exemplare, Platz 1 der Bestenliste in Frankreich
-Die Rechte wurden bereits in 26 Länder verkauft
-Ein Roman über den einflussreichsten Berater von Putin und die mediale Inszenierung der Macht
-Basiert auf der realen Gestalt von Putins Spindoktor Wladislaw Surkow</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>978-3-406-79993-8</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Buch</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Gebunden</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Beck</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>24.04.2023</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Breite 139 mm, Höhe 217 mm, Dicke 25 mmGewicht480 g</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>55652787</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Wo wir uns trafen</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>32.90</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Lundberg, SofiaDörries, MaikeÜbersetzungSchöps, KerstinÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Nur wahre Freundschaft berührt dein Herz ...
-Lidingö, Südschweden: Jeden zweiten Samstag sitzt die frisch geschiedene Esther auf einer Bank unter einer alten Eiche und schaut hinaus aufs Meer. Die Wochenenden, die ihr Sohn bei seinem Vater verbringt, sind schwer, und hier kann Esther ihren Gefühlen freien Lauf lassen. Eines Tages trifft sie dort auf Rut, eine alleinstehende, ältere Dame, die Esther mit ihrer warmherzigen Art tröstet. Zwischen den beiden Frauen entsteht eine tiefe Freundschaft, und die Bank am Meer wird zu ihrem regelmäßigen Treffpunkt. Doch dann verschwindet Rut, und als Esther sich auf die Suche nach ihr macht, kommt sie einer dramatischen Lebensgeschichte auf die Spur ...</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>978-3-442-31645-8</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Buch</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Gebunden</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Goldmann</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>26.04.2023</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1. A.</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Breite 148 mm, Höhe 221 mm, Dicke 37 mmGewicht564 g</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Going Zero</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>34.00</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Hat man als Einzelner überhaupt eine Chance gegen das System? Eine junge Bibliothekarin aus Boston ist entschlossen, es zu versuchen - ihr bleibt keine Wahl. Und so greift sie zu, als sich die Einladung zu einem ungewöhnlichen Kräftemessen bietet: dem Betatest von FUSION, einem Projekt der US-Geheimdienste und des Social-Media-Moguls Cy Baxter. Wem es gelingt, 30 Tage unauffindbar zu bleiben, dem winken 3 Millionen Dollar. Doch Kaitlyn geht es um etwas anderes.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>978-3-257-07192-4</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Buch</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Gebunden</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Diogenes</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>26.04.2023</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>1. A.</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
@@ -854,7 +871,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Breite 116 mm, Höhe 184 mm, Dicke 30 mmGewicht403 g</t>
+          <t>Breite 133 mm, Höhe 209 mm, Dicke 23 mmGewicht330 g</t>
         </is>
       </c>
       <c r="P6" t="inlineStr"/>
@@ -862,56 +879,56 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sommernächte in Paris</t>
+          <t>Die Krume Brot</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16.90</t>
+          <t>29.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Swan, KarenWittich, GertrudÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>belletristik schweizer</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ein unvergesslicher Sommer in der Stadt der Liebe ...
-Die Kunstagentin Flora Sykes ist ständig in der Welt unterwegs. Für ein Privatleben oder eine ernsthafte Beziehung bleibt da keine Zeit. Nun führt sie ein geheimnisvoller Auftrag nach Paris, wo die wohlhabende Familie Vermeil ein Apartment voller Kunstschätze geerbt hat, das seit über siebzig Jahren niemand mehr betreten hat. Warum war es so lange verschlossen? Und woher stammen die Bilder? Statt Antworten zu finden, stößt Flora bei ihren Nachforschungen auf immer mehr Geheimnisse. Und zu allem Überfluss lenkt Xavier Vermeil, der unverschämt gut aussehende Sohn der Erben, sie immer wieder von der Arbeit ab ...</t>
+          <t>Adelina, Tochter italienischer Einwanderer, arbeitet in einer Zürcher Fabrik, als sie nach kurzem Liebesglück mit einem Kind allein dasteht. Sie verliert die Stelle, die Wohnung, kämpft ums Überleben. In der größten Not lernt sie Emil kennen, einen erfolgreichen Grafiker, der ihre Schulden bezahlt und Adelina mit der kleinen Emma bei sich aufnimmt. Außer an der Liebe fehlt es an nichts. Emil kauft ein Anwesen in den Bergen des Piemont und scheint auf gemeinsames Glück zu hoffen. Aber dann verschwindet das Kind, spurlos.
+Adelina macht sich auf die Suche, begleitet von einem schweigsamen Unbekannten. Er bringt sie nach Mailand, in eine Kommune, zu Menschen, die an die Revolution glauben und Adelina versprechen, die verlorene Tochter zu finden; sie muss nur bereit sein, sich dem Kampf anzuschließen, und mit ihren Schweizer Papieren über die Grenze gehen, auf eine gefährliche Mission.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>978-3-442-49396-8</t>
+          <t>978-3-498-00320-3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Taschenbuch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Goldmann</t>
+          <t>Rowohlt</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Deutsche Erstausgabe</t>
-        </is>
-      </c>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
@@ -921,7 +938,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Breite 126 mm, Höhe 187 mm, Dicke 35 mmGewicht394 g</t>
+          <t>Breite 133 mm, Höhe 209 mm, Dicke 23 mmGewicht330 g</t>
         </is>
       </c>
       <c r="P7" t="inlineStr"/>
@@ -929,29 +946,34 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>One of the Girls</t>
+          <t>Anuschka und Finn</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24.90</t>
+          <t>20.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Clarke, LucyHofstetter, UrbanÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>Schawinski, Roger</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>fachbuecher geschichte schweiz</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Sechs Frauen. Sechs Geheimnisse. Eine Leiche.
-Es sollte der perfekte Kurzurlaub werden: Lexi reist mit fünf Freundinnen auf eine griechische Insel, um ihren Junggesellinnenabschied zu feiern. Von der abgelegenen Villa mit Meerblick bis hin zu den malerischen Tavernen und weiß getünchten Straßen scheint der Urlaub zu schön, um wahr zu sein. Und tatsächlich bekommt die Idylle bald Risse, denn abgesehen von ihrer Freundschaft mit Lexi haben die Frauen nur eines gemeinsam: Sie alle haben etwas zu verbergen. Nach und nach kommen versteckte Absichten ans Licht, Geheimnisse werden enthüllt und die Masken fallen - bis eine Leiche auf den Klippen unterhalb der Villa liegt...</t>
+          <t>Roger Schawinski über einen Medienskandal, der nicht nur die Schweiz bewegte. Ab 12. Mai im Buchhandel erhältlich.
+Im Spiegel beschuldigte die renommierte Journalistin Anuschka Roshani ihren ehemaligen Chef und Freund Finn Canonica beim Magazin (Tages-Anzeiger) aufs Heftigste. Er habe sie mit Sexismus, Mobbing und Machtmissbrauch gequält. "Rund 14 Jahre lang versuchte ich ihm zu entkommen", hielt sie in ihrem "Gastbeitrag" fest und belegte dieses vernichtende Urteil mit einer Vielzahl von konkreten Beispielen. Tamedia hat inzwischen Klage gegen den Spiegel eingereicht, Tamedia hält Text und Bilder für persönlichkeitsverletzend.
+In diesem Buch werden die Hintergründe dieses Falls beleuchtet, der in der Schweiz und in Deutschland hohe Wellen geworfen hat. Was stimmt an den Vorwürfen und was nicht? Was wurde bewiesen und was widerlegt? Wie hatte es überhaupt zu dieser Affäre kommen können? Und wie gehen die Medien in der aktuell aufgeheizten Gender-Diskussion mit einem solchen Thema um? Die Antworten zu diesen Fragen sind überraschend und beängstigend zugleich. Radio 1 - Chef Roger Schawinski, ein ausgezeichneter Kenner der deutschsprachigen Medienlandschaft, veröffentlicht nun im Radio-1-Verlag seinen Blick auf den Skandal und den Umgang der Medien damit.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>978-3-423-26359-7</t>
+          <t>978-3-033-09890-9</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -966,12 +988,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>DTV</t>
+          <t>Radio 1 AG</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
+          <t>12.05.2023</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -984,15 +1006,19 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Breite 136 mm, Höhe 210 mm, Dicke 31 mmGewicht450 g</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr"/>
+          <t>Breite 144 mm, Höhe 221 mm, Dicke 15 mmGewicht272 g</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>58408389</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Liebe oder Eierlikör - Fast eine Romanze</t>
+          <t>Elternabend</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1002,19 +1028,25 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Heldt, Dora</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>Fitzek, Sebastian</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Früher war mehr Romantik ...
-Ernst Mannsen versteht die Welt nicht mehr. Die sonst so verlässliche Hilke Petersen trägt plötzlich Lippenstift und hat keine Zeit, auf dem Frühlingsbazar Kuchen zu verkaufen. Hella und Gudrun reden von Frühlingsgefühlen und Liebeshormonen und vermuten, dass Hilke eine Romanze hat. Und plötzlich taucht auch noch das Gerücht auf, dass das halbe Dorf sich bei einer Dating-App angemeldet hat, die Liebe oder Eierlikör heißt. Und das, obwohl Ernst schon so viel über Betrüger im Netz gelesen hat. Er vermutet, dass der Lippenstift nur der Anfang der Katastrophe ist, in die Hilke sich begibt, und ist entschlossen, das zu verhindern. Mithilfe seines Enkels Mats und Freundin Hella forscht er undercover nach, nicht ahnend, wie schnell man sich auf einem Date wiederfinden kann ...</t>
+          <t>Stell dir vor ...
+... du musst eine halbe Ewigkeit auf einem Elternabend verbringen. Dabei hast du gar kein Kind!
+Ein lebenskluger und hinreißend komischer Roman im Stil von Sebastian Fitzeks Nr.1-Bestseller »Der erste letzte Tag«
+Sascha Nebel hat sich zur falschen Zeit am falschen Ort das falsche Auto für einen Diebstahl ausgesucht. Kaum, dass er hinter dem Steuer eines Geländewagens Platz genommen hat, zieht eine Horde demonstrierender Klimaaktivisten durch die Straße. Allen voran eine junge Frau, die den SUV mit einer Baseballkeule demoliert. Als die Polizei auf der Bildfläche erscheint, ergreifen Sascha und die Unbekannte die Flucht und platzen in den Elternabend einer 5. Klasse. Um die Nacht nicht in Polizeigewahrsam zu verbringen, bleibt ihnen keine andere Wahl: Sie müssen in die Rolle von Christin und Lutz Schmolke schlüpfen, den Eltern des 11jährigen Hector, die bislang jede Schulveranstaltung versäumten. Zwei wildfremde Menschen, zwischen denen kaum größeres Streitpotential herrschen könnte, geben sich als Vater und Mutter eines ihnen völlig unbekannten Kindes aus. Dabei ist die Tatsache, dass Hector der größte Rüpel der Schule ist, sehr schnell ihr kleinstes Problem ...</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>978-3-423-28337-3</t>
+          <t>978-3-426-28413-1</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1024,17 +1056,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Gebunden</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>DTV</t>
+          <t>Droemer/Knaur</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
+          <t>26.04.2023Erstverkaufstag26.04.2023</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1047,7 +1079,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Breite 119 mm, Höhe 175 mm, Dicke 24 mmGewicht280 g</t>
+          <t>Breite 135 mm, Höhe 210 mm, Dicke 25 mm</t>
         </is>
       </c>
       <c r="P9" t="inlineStr"/>
@@ -1055,28 +1087,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Damals im Tessin</t>
+          <t>Troubadour</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>26.90</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+          <t>Walker, MartinWindgassen, MichaelÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Zwanzig Jahre sind vergangen, seit Malvaglia, ein kleines Dorf in den Tessiner Bergen, geflutet wurde, um auf dem Gelände einen Stausee entstehen zu lassen. Beinahe haben die einstigen Bewohner, deren Häuser damals unter Wasser gesetzt wurden, das Unrecht vergessen. Besonders der verschlossene Privatdetektiv Elia Contini, der zurückgezogen in einem Häuschen in den Bergen wohnt und am liebsten durch die Wälder streift, um Füchse zu fotografieren, denkt ungern an die Zeit zurück, in der sein Vater unter ungeklärten Umständen verschwand. Doch jetzt soll der Stausee erweitert und jener Teil des Sees trockengelegt werden, auf dem auch das Haus seiner Kindheit stand. Alte Wunden brechen auf. Als kurz hintereinander der Bürgermeister und ein Ingenieur ermordet werden, gerät Contini ins Fadenkreuz der Ermittler. Um sich selbst zu entlasten, muss er sich endlich der Vergangenheit stellen und herausfinden, was damals wirklich geschah ...</t>
+          <t>Bruno steckt mitten in den Vorbereitungen für das alljährliche Konzert in Saint-Denis - die Folkband Les Troubadours soll auftreten, die mit ihrem neuesten Hit 'A Song for Catalonia' gerade in Spanien für Zündstoff sorgt. Hinweise auf einen geplanten Mordanschlag werden laut. Doch Bruno hat auch anderweitig alle Hände voll zu tun: Er ist zuständig für das Buffet eines Tennisturniers, ein Wildschwein wird über offenem Feuer gebraten, es wird gefeiert und geschlemmt - aber ist es Zufall, dass plötzlich vier junge Tennisasse aus Katalonien so viele Spiele für sich entscheiden?</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>978-3-7152-5503-3</t>
+          <t>978-3-257-07237-2</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1086,63 +1122,70 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Atlantis Zürich</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>n-Nr.15</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>Breite 125 mm, Höhe 205 mm, Dicke 33 mmGewicht396 g</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>55771950</t>
-        </is>
-      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Die Schweiz und ihre Neutralität</t>
+          <t>Der Magier im Kreml</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>49.00</t>
+          <t>36.90</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jorio, Marco</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>Da Empoli, GiulianoMeßner, MichaelaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Die Schweiz sucht ihre Rolle in Europa und der Welt nicht erst seit dem Ausbruch des Kriegs in der Ukraine. Mit dem schrittweisen Aufbau der Europäischen Union und dem Ende des Kalten Krieges (1989) hat sich die internationale Lage unseres Landes von Grund auf geändert. Die Schweiz muss sich überlegen, welche Haltung sie als Staat mitten in Europa einnimmt und wie sie sich nach dem Untergang der bipolaren Welt positioniert. In diesen Diskussionen spielt die Neutralität eine zentrale Rolle. Aus der Staatsmaxime ist ein nationales Identitätsmerkmal geworden. Woher kommt diese tiefe Verankerung in der Bevölkerung? Wie konnte die Neutralität die Identität des Landes dermassen prägen? Wie, wann und warum entstand sie? Und können aus der Vergangenheit Perspektiven für die Zukunft aufgezeigt werden?Der Blick auf 400 Jahre Neutralitätsgeschichte gibt Antworten auf diese Fragen. 50 Jahre nach dem monumentalen Werk von Edgar Bonjour (1965-1970) legt der Historiker Marco Jorio eine neue Gesamtdarstellung zum Thema auf der Basis der Forschungen der letzten Jahrzehnte vor.</t>
+          <t>SPIEGEL-BESTSELLER UND VIELFACH AUSGEZEICHNET
+Man nennt ihn den «Magier im Kreml». Der rätselhafte Vadim Baranow war Regisseur und Produzent von Reality-TV-Shows, bevor er zur grauen Eminenz von Putin wird. Nachdem er als politischer Berater von der Bühne verschwindet, werden immer mehr Legenden über ihn verbreitet. Bis er eines Nachts dem Ich-Erzähler dieses Buches, der seit Langem in Moskauer Archiven forscht, seine Geschichte anvertraut ...
+Dieser Roman führt uns ins Zentrum der russischen Macht, wo permanent Intrigen gesponnen werden. Und wo Vadim, der zum wichtigsten Spindoktor des Regimes geworden ist, ein ganzes Land in ein politisches Theater verwandelt, in dem es keine andere Realität als die Erfüllung der Wünsche des Präsidenten gibt. Doch Vadim ist kein gewöhnlicher Ehrgeizling: Der Regisseur, der sich unter die Wölfe verirrt hat, gerät immer tiefer in die Machenschaften des Systems, das er selbst mit aufgebaut hat, und wird alles daransetzen, um dort wieder herauszukommen. Er nimmt den Erzähler mit auf eine Reise ins Herz der Finsternis. «Der Magier im Kreml» ist ein großer Roman über das zeitgenössische Russland und die Entstehung seiner medial inszenierten und vollkommen fiktiven, aber auch tödlichen Realität, einem Imperium der Lüge. Er enthüllt nicht nur die Hintergründe der Putin-Ära, sondern bietet auch eine hellsichtige Betrachtung über die Macht.
+Ausgezeichnet mit dem Grand Prix du Roman de l'Académie française Finalist des Prix Goncourt 2022 200 000 verkaufte Exemplare, Platz 1 der Bestenliste in Frankreich Die Rechte wurden bereits in 26 Länder verkauft Ein Roman über den einflussreichsten Berater von Putin und die mediale Inszenierung der Macht Basiert auf der realen Gestalt von Putins Spindoktor Wladislaw Surkow</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>978-3-03919-389-9</t>
+          <t>978-3-406-79993-8</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1157,12 +1200,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>hier + jetzt</t>
+          <t>Beck</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>15.04.2023</t>
+          <t>24.04.2023</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1175,36 +1218,49 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Breite 160 mm, Höhe 240 mm, Dicke 33 mmGewicht1134 gIllustrationenca. 20 sw und farbige Abbildungen</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr"/>
+          <t>Breite 139 mm, Höhe 217 mm, Dicke 25 mmGewicht480 g</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>55652787</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Der Campingplatzkiller</t>
+          <t>Noch wach?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>25.90</t>
+          <t>34.50</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>Stuckrad-Barre, Benjamin von</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Camping erfreut sich immer großerer Beliebtheit. Statt spießiger Kleinbürgeridylle ist das »Vanlife« auch in der jüngeren Generation angekommen: Ausgebuchte Platze, in der Hauptsaison sogar Wartelisten. Für die Dauercamper sind Touristen unerwünschte Eindringlinge in ihr Paradies. Heinrich »Henry« Kummer ist nicht ganz freiwillig auf dem Campingplatz gelandet. Mit 60 hat er seine Frühpensionierung beantragt - »So einen Bauchschuss lasst einen nachdenken«. Polizist war er, 32 Jahren lang. Aber keiner, der Verbrecher jagt, nicht einmal einer, der den Verkehr regelt. Als sich ihm die Gelegenheit geboten hat, ließ er sich in den Hausdienst versetzen. Und ist hangen geblieben. 25 Jahre hat er am Empfang des Kripo-Gebaudes in der Zürcher Kasernenstrasse verbracht. War für den Hausdienst zustandig, eine Art Abwart oder Portier. Und doch wurde ausgerechnet er bei einem Einsatz lebensgefahrlich verletzt. Aber auch das war keine Heldentat: Er war nur zur falschen Zeit am falschen Ort. Kummers neues Leben auf vier Radern beginnt weniger erholsam als gedacht: Dauercamperin Rosa wird tot in ihrem Wohnwagen gefunden: durchgeschnittene Kehle, ein einziger, sauberer Schnitt. Kummer ware nicht sein halbes Leben Polizist gewesen, wenn er den Ermittlungen tatenlos vom Campingstuhl aus zusehen würde ...</t>
+          <t>Berlin: Eine junge Frau erzählt von ihrem neuen Job bei einem großen Fernsehsender, von ihrem neuen Chef, ihrem neuen Leben. Sie wirkt glücklich, beseelt, hoffnungsfroh, es klingt gut. Zu gut?
+In Los Angeles geht derweil eine Welt unter. Ein Mann, der damit prahlt, als Berühmtheit könne man sich gegenüber Frauen alles herausnehmen, wird Präsident der Vereinigten Staaten. Im Garten des legendären "Chateau Marmont", diesem Nachtspielplatz verwöhnter Hollywood Kids jeden Alters, vertreibt sich eine illustre Bande auf der Flucht vor der Realität die Zeit. Auch der Erzähler ist hier - und Rose McGowan, die Schauspielerin, der man nachsagt, neuerdings irgendwie anstrengend geworden zu sein.
+Kurz darauf erschüttert der Weinstein-Skandal Hollywood, und Rose McGowan ist eine der ersten Frauen, die sexuelle Belästigung durch den bis dahin von ganz Hollywood hofierten Filmproduzenten öffentlich gemacht hat. Rose verschwindet, aber sie hinterlässt dem Erzähler eine kryptische Nachricht - oder ist es vielmehr ein Auftrag? Wieso wendet sie sich ausgerechnet an ihn?
+Von Hollywood aus verbreitet sich die #MeToo-Bewegung um die ganze Welt. Doch die alten Machtstrukturen sind widerständiger, als man in der ersten Euphorie vielleicht denken mochte.
+Zurück in Berlin findet sich der Erzähler nicht mehr nur als Liegestuhlbeobachter, sondern nun als Akteur mitten in einem unübersichtlichen Geschehen wieder, das ihn in einen tiefen persönlichen Konflikt stürzt.
+"Noch wach?" ist ein Sittengemälde unserer Zeit, ein typischer Stuckrad-Barre. Literarisch brillant, humorvoll und kompromisslos erzählt dieser Roman von Machtstrukturen und Machtmissbrauch, Mut und menschlichen Abgründen.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>978-3-7152-5506-4</t>
+          <t>978-3-462-00467-0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1214,17 +1270,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Atlantis Zürich</t>
+          <t>Kiepenheuer &amp; Witsch</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
+          <t>19.04.2023</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1237,60 +1293,64 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Breite 125 mm, Höhe 205 mm, Dicke 25 mmGewicht270 g</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>55898510</t>
-        </is>
-      </c>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 34 mmGewicht499 g</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Die Mitternachtsrose</t>
+          <t>Der letzte Sessellift</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17.90</t>
+          <t>45.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Riley, LucindaHauser, SonjaÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Innerlich aufgelöst kommt die amerikanische Schauspielerin Rebecca Bradley im englischen Dartmoor an, wo ein altes Herrenhaus als Kulisse für einen Film dient, der in den 1920er Jahren spielt. Vor ihrer Abreise hat die Nachricht von Rebeccas angeblicher Verlobung eine Hetzjagd der Medien auf die junge Frau ausgelöst, doch in der Abgeschiedenheit von Astbury Hall kommt Rebecca allmählich zur Ruhe. Als sie jedoch erkennt, dass sie Lady Violet, der Großmutter des Hausherrn, frappierend ähnlich sieht, ist ihre Neugier geweckt. Dann taucht Ari Malik auf: ein junger Inder, den das Vermächtnis seiner Urgroßmutter Anahita nach Astbury Hall geführt hat. Und gemeinsam kommen sie nicht nur Anahitas Geschichte auf die Spur, sondern auch dem dunklen Geheimnis, das wie ein Fluch über der Dynastie der Astburys zu liegen scheint ...</t>
+          <t xml:space="preserve"> 
+»Es gibt mehr als nur eine Art, jemanden zu lieben.«
+Aspen, Colorado 1941. Mit 18 tritt Rachel Brewster bei den nationalen Skimeisterschaften an. Eine Medaille gibt es nicht, dafür ist sie schwanger, als sie in ihre Heimat Exeter in New Hampshire zurückkehrt. Fortan arbeitet sie als Skilehrerin und verbringt das halbe Jahr in Vermont, weshalb ihr Sohn Adam bei seiner Großmutter Nana aufwächst.
+Adams Großvater hat aufgehört zu sprechen, als er die Nachricht von der unehelichen Schwangerschaft seiner jüngsten Tochter Rachel erhält, und rutscht unaufhaltsam in eine Demenz. Rachels Schwestern Abigail und Martha bevölkern ebenfalls Adams Welt und kommentieren wie ein griechischer Chor voller Missbilligung alles, was Rachel und Adam tun. Als Adam 14 ist, verkuppelt er die 1,57 m kleine Rachel mit dem noch kleineren Englischlehrer Mr. Barlow, einem Schneeschuhläufer. Und obwohl Großvater Lew während der Hochzeit eine Beißattacke auf die Knöchel der Gäste unternimmt, obwohl er wenig später nur in Windeln vom Blitz erschlagen wird, obwohl Rachel Mr. Barlow in derselben Nacht mit ihrer Lebensgefährtin Molly betrügt, wird aus Rachel, Adam und Elliot Barlow eine Familie, in deren Schutz jedes Mitglied seinen Neigungen nachgehen kann: Adam wird Drehbuchautor, Rachel frönt dem Skifahren und Molly, Mr. Barlow trägt Frauenkleider.
+Doch Irving wäre nicht Irving, wenn es nicht auf diesem Höhepunkt steil abwärts gehen würde: Morde geschehen und Selbstmorde, Hass, Neid und Missgunst zerstören den Seelenfrieden der Charaktere, die Gesellschaft stößt diejenigen aus, die nicht konform sein wollen. Zum Glück versöhnt uns Irving mit einem friedvollen Ende für Adam, der uns sein Leben von seiner Geburt bis ins sehr hohe Alter erzählt.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>978-3-442-49429-3</t>
+          <t>978-3-257-07222-8</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Taschenbuch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Goldmann</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1307,7 +1367,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Breite 128 mm, Höhe 188 mm, Dicke 39 mmGewicht440 g</t>
+          <t>Breite 116 mm, Höhe 184 mm, Dicke 55 mmGewicht744 g</t>
         </is>
       </c>
       <c r="P13" t="inlineStr"/>
@@ -1315,34 +1375,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Das kleine WIR in der 1. Klasse</t>
+          <t>Sturz in die Sonne</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>13.90</t>
+          <t>30.00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Herrenbrück, AnjaKunkel, Daniela</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>Ramuz, Charles FerdinandWyss, StevenÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>belletristik schweizer</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Schulanfang und das kleine WIR
-Auch die Kinder der ersten Klasse haben ein kleines WIR. Ob Matheunterricht, Lesen und Schreiben, Sport oder große Pause - mit dem WIR macht alles doppelt so viel Spaß. Doch die Schüler_innen der Wolkenklasse sind nicht immer einer Meinung. Sie haben auch mal Streit oder sagen blöde Sachen. Dann verschwindet das kleine WIR, und die Kinder vermissen es sehr. Denn ohne WIR-Gefühl fehlt der Wolkenklasse der Zusammenhalt. Zum Glück wissen die Schüler_innen, wie sie ihr WIR aufstöbern und aufpäppeln können. Bald ist ihr kleines WIR groß und stark. Und eins ist klar: Gemeinsam ist es einfach am schönsten!
-Unterstützt Kinder beim Lösen von KonfliktenEmpowert Kinder, füreinander da zu sein und gegen Ausgrenzung einzustehenAnschaulich und erstlesefreundlich erzähltGeeignet für Vor- und Grundschüler_innen
-Einfach Lesen lernen:
-1. Lesestufe: große Fibelschrift, leichte Wörter Kleine Texteinheiten in Kombination mit vielen bunten BildernComicelemente, um die Sehgewohnheiten von Kindern zu berücksichtigen
-lebensnahe Geschichte aus dem Kinderalltag
-Freundschaft, Zusammenhalt und WIR-Gefühl: ein wichtiges Thema, besonders für Erstlesekinder in der 1. Klasse. Das beliebte kleine WIR, jetzt auch zum ersten Lesen!</t>
+          <t>Am Anfang steht eine wissenschaftliche Entdeckung: Wegen eines Unfalls im Gravitationssystem stürzt die Erde in die Sonne zurück. «Es wird immer heißer werden und schnell wird alles sterben», schreibt C.F. Ramuz lakonisch dazu. Die Menschen am Ufer des Genfersees wollen das erst nicht glauben und erfreuen sich am schönen Wetter. Aber schnell wird klar, dass es vor der Hitze keine Entkommen gibt. 1922, als der Roman erstmals erschien, wusste C.F. Ramuz noch nichts von der Bedrohung der globalen Erwärmung, der wir heute gegenüberstehen. Doch das düstere Bild, das er in diesem visionären Text in seiner einzigartig verdichteten Sprache zeichnet, liest sich wie eine Prophezeiung.«Eine echte Trouvaille, das beste Beispiel für die Kraft der Literatur: Mit Sprache und Imagination schafft Ramuz eine eigene Welt und leuchtet ins Wesen der Menschen hinein.» NZZ</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>978-3-551-69026-5</t>
+          <t>978-3-03926-055-3</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1355,14 +1413,10 @@
           <t>Gebunden</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Carlsen</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>27.04.2023</t>
+          <t>08.05.2023</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1375,36 +1429,47 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Breite 160 mm, Höhe 215 mm, Dicke 15 mmGewicht286 gIllustrationenFarb. Abb.</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr"/>
+          <t>Breite 115 mm, Höhe 190 mm, Dicke 30 mmGewicht256 g</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>55828942</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Idefix und die Unbeugsamen - Der Wecker von Lutetia - Erstlesebuch zur Serie</t>
+          <t>Das Café ohne Namen</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16.90</t>
+          <t>34.90</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Uderzo, RenéGoscinny, AlbertJöken, KlausÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+          <t>Seethaler, Robert</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>In Lutetia stimmt etwas nicht. Alle Gallier haben verschlafen. Wo ist nur Sinfonix, der Hahn, dessen donnerndes Kikiriki sie normalerweise aus dem Schlaf reißt? Wurde er vielleicht von den Römern entführt? Idefix und seine Freunde müssen der Sache rasch auf den Grund gehen, bevor ihr Freund als Brathähnchen endet!Die Abenteuer von Idefix nacherzählt zum eingenständigen lesen, mit vielen Bildern aus der TV-Serie!</t>
+          <t>Ein Café und seine Menschen. Ein Mann, der seiner Sehnsucht folgt. Robert Seethalers neuer Roman.
+Wien im Jahr 1966. Robert Simon verdient sein Brot als Gelegenheitsarbeiter auf dem Karmelitermarkt. Er ist zufrieden mit seinem Leben, doch zwanzig Jahre nach Ende des Krieges hat sich die Stadt aus ihren Trümmern erhoben. Überall wächst das Neue, und auch Simon lässt sich mitreißen. Er pachtet eine Gastwirtschaft und eröffnet sein eigenes Café. Das Angebot ist überschaubar, und genau genommen ist es gar kein richtiges Café, doch die Menschen aus dem Viertel kommen, und sie bringen ihre Geschichten mit - von der Sehnsucht, vom Verlust, vom unverhofften Glück. Sie kommen auf der Suche nach Gesellschaft, manche hoffen sogar auf die Liebe, und während die Stadt um sie herum erwacht, verwandelt sich auch Simons eigenes Leben.
+Das Café ohne Namen ist ein Roman über den menschlichen Drang zum Aufbruch. Mit einem Reigen unvergesslicher Figuren und seiner besonderen Aufmerksamkeit für die Details des Lebens erzählt Robert Seethaler davon, wie eine neue Welt entsteht, die wie alles Neue ihr Ende schon in sich trägt.
+"Niemand muss Robert Seethaler lesen, um zu begreifen, dass das Scheitern die zentrale Erfahrung des Lebens ist. Aber man liest davon bei Seethaler nach wie vor lieber als anderswo, weil er so behutsam davon zu erzählen versteht, ohne größere Ausflüchte oder Umwege." Cornelius Pollmer, Süddeutsche Zeitung</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>978-3-7704-0731-6</t>
+          <t>978-3-546-10032-8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1417,14 +1482,10 @@
           <t>Gebunden</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Ehapa Comic Collection</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>08.05.2023</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1437,41 +1498,43 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Breite 153 mm, Höhe 216 mm, Dicke 10 mmGewicht304 g</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>55687597</t>
-        </is>
-      </c>
+          <t>Breite 128 mm, Höhe 210 mm, Dicke 28 mmGewicht386 g</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Trügerische Provence</t>
+          <t>Mit dem Mut zur Liebe</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17.90</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Lagrange, Pierre</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
+          <t>Lind, Hera</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Ein trügerischer Festspiel-Sommer in der Provence - der siebte Band der Provence-Krimi-Reihe von Bestseller-Autor Pierre Lagrange
-Mitten in der Konzertsaison in der Provence verschwinden plötzlich namhafte Musikerinnen. Die Ermittlungskommission unter Leitung von Caterine Castel und Alain Theroux tappt im Dunkeln. Es gibt keine Hinweise oder Forderungen im Zusammenhang mit der Entführung. Obwohl Ex-Commissaire Albin Leclerc mitten in den eigenen Hochzeitsvorbereitungen steckt, kann er es mal wieder nicht lassen: zusammen mit seinem Mops Tyson nimmt er die Spur auf. Als es zu einer weiteren Entführung kommt, und auch die kostbaren Instrumente verschwinden, stellt sich für ihn die Frage, ob in der Provence ein Wahnsinniger unterwegs ist. Die Ermittlungen bringen Albin Leclerc in allergrößte Gefahr ...</t>
+          <t>Erst ein dramatischer Unfall, dann die waghalsige Flucht aus der DDR:
+Im Tatsachenroman »Mit dem Mut zur Liebe« erzählt Nummer-1-Bestseller-Autorin Hera Lind die wahre Liebesgeschichte der Artisten Dieto und Johanna.
+Es ist Liebe auf den ersten Blick, als sich Johanna und Dieto 1957 in Dresden zum ersten Mal begegnen. Ihre Väter waren zusammen in russischer Kriegsgefangenschaft, und beide bringen ihren Kindern die artistischen Kunststücke bei, die ihnen den sicheren Tod im Arbeitslager erspart haben. Doch als das junge Artistenpaar nach hartem Drill schließlich Weltniveau erreicht, muss Dieto sich drei Jahre beim Militär verpflichten. Das junge Paar flieht Hals über Kopf in einem Schlauchboot über die Adria, wo sie nur mit Badesachen bekleidet nach 36 Stunden völlig erschöpft ankommen .Da wird ihnen bewusst, dass sie ohne ihr Equipmentkeine Existenz aufbauen können. Dieto lässt Johanna bei Fremden zurück und versucht es ein zweites Mal....
+Ergreifend und voller Hoffnung erzählt der dramatische Tatsachenroman von Bestseller-Autorin Hera Lind die wahre Geschichte eines ganz normalen Paares aus der DDR, dessen Liebe über alle Grenzen trägt.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>978-3-596-70646-4</t>
+          <t>978-3-426-52840-2</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1486,61 +1549,74 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>FISCHER Taschenbuch</t>
+          <t>Droemer/Knaur</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>26.04.2023</t>
+          <t>02.05.2023</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>n-Nr.07</t>
-        </is>
-      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Breite 125 mm, Höhe 190 mm, Dicke 36 mmGewicht441 g</t>
+        </is>
+      </c>
       <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Every (deutsche Ausgabe)</t>
+          <t>Gnadenlose Provence</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>22.90</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Eggers, DaveTimmermann, KlausÜbersetzungWasel, UlrikeÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
+          <t>Lagrange, Pierre</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Der Circle ist die größte Suchmaschine gepaart mit dem größten Social-Media-Anbieter der Welt. Eine Fusion mit dem erfolgreichsten Onlineversandhaus brachte das reichste und gefährlichste - und seltsamerweise auch beliebteste - Monopol aller Zeiten hervor: Every.
-Delaney Wells ist »die Neue« bei Every und nicht gerade das, was man erwarten würde in einem Tech-Unternehmen. Als ehemalige Försterin und unerschütterliche Technikskeptikerin bahnt sie sich heimlich ihren Weg, mit nur einem Ziel vor Augen: die Firma von innen heraus zu zerschlagen. Zusammen mit ihrem Kollegen, dem nicht gerade ehrgeizigen Wes Kavakian, sucht sie nach den Schwachstellen von Every und hofft, die Menschheit von der allumfassenden Überwachung und der emojigesteuerten Infantilisierung zu befreien. Aber will die Menschheit überhaupt, wofür Delaney kämpft? Will die Menschheit wirklich frei sein?
-Wie schon bei »Der Circle« weiß Dave Eggers wie kein Zweiter unsere Wirklichkeit so konsequent weiterzudenken, dass einem der Atem stockt beim Lesen. Man kann nur inständig hoffen, dass die Realität nicht schneller voranschreitet, als Dave Eggers schreiben kann.</t>
+          <t>Eine gnadenlose Tat erschüttert die Provence - der achte Band der Provence-Krimi-Reihe von Bestseller-Autor Pierre Lagrange
+Zahllose Radsportler sausen im Sommer durch die Provence - und ein Scharfschütze zieht einen nach dem anderen aus dem Verkehr. Die Ermittler Castel und Theroux sind geschockt und haben keinen Schimmer, um wen es sich bei dem Täter handeln könnte. Albin Leclerc, Commissaire im Ruhestand, erfährt von den Vorfällen, während er seine Flitterwochen auf Martinique verbringt. Kaum zurück, stürzt er sich in die Ermittlungen. Er befürchtet, dass der Schütze sich bisher nur aufwärmt und es auf die Tour de France abgesehen hat, die in Kürze durch Carpentras führen wird. Ein Rennen um Leben und Tod beginnt, bei dem sich herausstellt: Die Hintergründe sind finsterer als gedacht ...
+Ex-Commissaire Albin Leclerc ermittelt in der Provence: die Provence-Krimi-Reihe
+Band 1: Tod in der Provence
+Band 2: Blutrote Provence
+Band 3: Mörderische Provence
+Band 4: Schatten der Provence
+Band 5: Düstere Provence
+Band 6: Eiskalte Provence
+Band 7: Trügerische Provence
+Band 8: Gnadenlose Provence
+Band 9: Unheilvolle Provence</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>978-3-462-00442-7</t>
+          <t>978-3-651-02592-9</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Taschenbuch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1550,66 +1626,62 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Kiepenheuer &amp; Witsch</t>
+          <t>FISCHER Scherz</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>04.05.2023</t>
+          <t>26.04.2023</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>n-Nr.08</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>Breite 126 mm, Höhe 191 mm, Dicke 25 mmGewicht374 g</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Pferdeflüsterer-Academy, Band 12: Wild und verwundbar</t>
+          <t>Die unfassbare Vielfalt des Seins</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>41.90</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mayer, Gina</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+          <t>Bridle, JamesWirthensohn, AndreasÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>fachbuecher biologie</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Im wilden Kanada steht ein weißes Schloss: Snowfields. Auf dem Internat werden die weltbesten Reiter ausgebildet und verletzte Pferdeseelen geheilt.
-Zwei Neue in Snowfields sorgen für Liebeschaos pur. Der attraktive Schüler Petter, zu dem sich Zoes Freundin Isabelle stark hingezogen fühlt. Und die junge Lehrerin, die bei einigen Lehrkräften heftigste Gefühle auslöst. Doch auch auf anderer Ebene herrscht Chaos. Im Internet kursieren schlimme Gerüchte über den Pferdeflüsterer Caleb. Und so langsam beschleicht Zoe das Gefühl, dass das nicht alles nur Lügen sind ...
-Entdecke alle Abenteuer an der "Pferdeflüsterer-Academy":
-Band 1: Reise nach Snowfields
-Band 2: Ein geheimes Versprechen
-Band 3: Eine gefährliche Schönheit
-Band 4: Verletztes Vertrauen
-Band 5: Zerbrechliche Träume
-Band 6: Calypsos Fohlen
-Band 7: Flammendes Herz
-Band 8: Zoes größter Sieg
-Band 9: Cyprians Rückkehr
-Band 10: Die dunkle Wahrheit</t>
+          <t>AUF DER SUCHE NACH DER PLANETARISCHEN INTELLIGENZ - DAS NEUE BUCH VON JAMES BRIDLE
+Intelligent ist nicht nur das, was Menschen und manche Maschinen tun. Vielmehr sollten wir die beeindruckende, schier unfassbare Vielfalt von intelligenten Existenzformen auf unserem Planeten neu entdecken. Von Mimosen über Gibbons bis zu Krabbencomputern und Satelliten: James Bridle erzählt in seinem Buch eine radikal neue Geschichte über Ökologie, Technik und unsere geteilte Welt.
+Durch eine Überbewertung unserer eigenen menschlichen Intelligenz haben wir uns von anderen Existenzweisen derart abgekoppelt, dass wir in die akute Misere der zunehmenden Zerstörung unseres Planeten geraten sind. Schuld daran sind unsere gängigen Vorstellungen von Intelligenz und Technologie: Die fortschrittlichsten Maschinen und ambitioniertesten Unternehmungen sind sowohl vom Egoismus unserer Spezies als auch von einer auf Profit und Extraktion ausgerichteten Denkweise tief geprägt. Um unsere Beziehung zum Rest des Planeten wieder sinnvoll zu gestalten, führt uns James Bridle auf eine grundlegend andere Ebene des Denkens und Erfahrens - eine Ebene, auf der wir überhaupt erst wieder in die Lage kommen, uns mit der überwältigenden Vielfalt von intelligenten Wesen um uns herum vertraut zu machen. Was können wir von ihnen lernen, und wie können wir unsere Gesellschaften verändern, um mit ihnen in eine florierende Gemeinschaft zu treten?
+Eine radikal neue Geschichte über Ökologie und Technik
+Theorie-Avantgarde im besten und verständlichen Sinn</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>978-3-473-40461-2</t>
+          <t>978-3-406-79895-5</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1622,22 +1694,22 @@
           <t>Gebunden</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Beck</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>01.05.2023</t>
+          <t>02.05.2023</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>1. Aufl.</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>HC - Pferdeflüsterer-Academy</t>
-        </is>
-      </c>
+          <t>3. A.</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
@@ -1646,7 +1718,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Breite 147 mm, Höhe 216 mm, Dicke 24 mm</t>
+          <t>Breite 139 mm, Höhe 217 mm, Dicke 35 mmGewicht702 g</t>
         </is>
       </c>
       <c r="P18" t="inlineStr"/>
@@ -1654,28 +1726,33 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Twisted Games</t>
+          <t>When You're Ready, This Is How You Heal</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>20.90</t>
+          <t>29.90</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Huang, AnaHallmann, MaikeÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
+          <t>Wiest, BriannaGraßtat, RenateÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>fachbuecher psychologie lebenshilfe</t>
+        </is>
+      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Sie ist eine Prinzessin. Er ihr Bodyguard. Ihr Beschützer. Ihr RuinGefangen von den Fesseln der Pflicht hat Bridget von Ascheberg, Prinzessin von Eldorra, nur drei Wünsche: Liebe, Leidenschaft und ihre eigenen Entscheidungen treffen zu dürfen. Doch als ihr Bruder seinen Anspruch auf den Thron aufgibt, findet sie sich auf einmal als zukünftige Königin wieder. Ein Titel, den sie nie wollte. An ihrer Seite der Mann, dem ihr Herz gehört, aber den sie nicht lieben darf: Rhys Larsen, ihr Bodyguard, ihr Beschützer, ihr Ruin. Ihre verbotenen Gefühle könnten sie beide in den Untergang treiben - und ihr Königreich zerstören.»Mitreißend, verboten und absolut süchtig machend - die Geschichte von Bridget und Rhys überzeugt mit einem perfekten Mix aus Gefühl, Leidenschaft und Tiefe.« CHARLEEN von CHARLIE_BOOKS Band 2 der heißen und romantischen TWISTED-Reihe von Bestseller-Autorin Ana Huang</t>
+          <t>Neue Essays der #1-Bestsellerautorin Brianna Wiest
+Schmerzhafte Ereignisse in unserem Leben können uns dauerhaft aus der Bahn werfen. Brianna Wiest zeigt in ihrem neuen Buch, wie wir uns selbst heilen können. Heilung bedeutet, den Schmerz zuzulassen und wirklich hinzusehen. Heilung bedeutet, sich auf eine Reise zu begeben, denn egal ob körperlich oder spirituell, sie verläuft weder linear noch nahtlos. Heilung bedeutet Verletzlichkeit. Heilung bedeutet, weiterzumachen, mit verwundetem, aber offenem Herzen. Heilung gelingt, wenn wir lernen, loszulassen, und den Mut finden, unser vergangenes Leben als das zu sehen, was es war, um unser jetziges Leben als das sehen zu können, was es ist: voller Hoffnung und Potenzial. Dieses Buch ist Balsam für jede Seele auf der Reise ihres eigenen Werdens.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>978-3-7363-1922-6</t>
+          <t>978-3-492-07161-1</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1685,25 +1762,21 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>LYX</t>
+          <t>Piper</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>28.04.2023</t>
+          <t>27.04.2023</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>n-Nr.02</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
@@ -1712,7 +1785,7 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Breite 135 mm, Höhe 215 mm, Dicke 41 mm</t>
+          <t>Breite 138 mm, Höhe 220 mm, Dicke 25 mmGewicht389 g</t>
         </is>
       </c>
       <c r="P19" t="inlineStr"/>
@@ -1720,30 +1793,34 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fußball Academy 3: Eine große Überraschung</t>
+          <t>Tom Gates - Ich bin dabei (wenn's gerade passt)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18.90</t>
+          <t>21.90</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Margil, IreneSchlüter, AndreasSaße, JanIllustrationen</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
+          <t>Pichon, LizKilchling, VerenaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>kids bis11</t>
+        </is>
+      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Training, Team und Tore - diesmal zusammen mit einer Mädchen-Fußballmannschaft!
-Yao und seine Freunde erleben in der Academy jeden Tag Training, Toreschießen und Türenknallen. Immer ist was los. Eines Tages ist das Fußball-Internat plötzlich voller Mädchen. Ein neues Team von jungen Fußballerinnen aus ganz Europa beginnt die Elite-Ausbildung. Und sie sind starke Spielerinnen! Die Jungs sind verunsichert. Sollen sie gegen Mädchen spielen? Können Mädchen eine Mannschaft sein? Schnell lernen sie Amanda, Maike, Nayara und die anderen kennen und respektieren. Eine schöne gemeinsame Zeit beginnt.
-Über Unterschiede und Gemeinsamkeiten von Jungs und Mädchen im FußballZeigt, wie man als Mannschaft wächstFrauenfußball bleibt Fußball!</t>
+          <t>Als Tom in einem Schaufenster die Deluxe-Box seiner Träume mit Kunst- und Zeichenutensilien entdeckt, kann er an NICHTS ANDERES mehr denken. Aber sein Geburtstag ist noch ewig hin und sein Sparschwein ist leer - Taschengeld anzusparen wird eine MILLION JAHRE dauern. Natürlich hat Tom schnell eine Idee: Er wird für ein bisschen Kleingeld den Nachbarn und seiner Familie beim Laub-Fegen, Auto-Waschen und anderem helfen. Doch die Dinge laufen schief, als er Delias Jeans schrumpft und die Unterwäsche seiner Mutter grau färbt ... Kann Tom das Geld für die Kunstbox auftreiben und trotzdem alle glücklich machen?
+Band 20 der Erfolgsserie
+Abwechslungsreich, kurzweilig und super witzig -für alle Comic-Fans ab 10 Jahren</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>978-3-551-65208-9</t>
+          <t>978-3-505-15049-4</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1758,18 +1835,22 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Carlsen</t>
+          <t>Schneiderbuch</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>27.04.2023</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
+          <t>25.04.2023</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>, Deutsche Erstausga</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>n-Nr.03</t>
+          <t>n-Nr.20</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
@@ -1778,17 +1859,13 @@
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>Breite 148 mm, Höhe 220 mm, Dicke 25 mm</t>
-        </is>
-      </c>
+      <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Man vergisst nicht, wie man schwimmt</t>
+          <t>Hard Land</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1798,19 +1875,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Huber, Christian</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>»Die einzige Möglichkeit, etwas vom Leben zu haben, ist, sich hineinzuwerfen.«
-31. August 1999. Sengende Hitze liegt über Bodenstein, dem Heimatkaff des 15-jährigen Pascal. Es sind die großen Ferien, und eigentlich könnte der Junge den Sommer genießen. Den Skatepark. Die Partys der Oberstufler. Das Freibad mit den besten Pommes des Planeten. Doch seit er nicht mehr schwimmen kann, mag Pascal den Sommer nicht mehr. Warum das so ist, das kann er nicht erzählen. Ebenso wenig, wieso ihn alle Krüger nennen. Und erst recht nicht, warum er sich unter keinen Umständen verlieben darf. Lieber träumt er vor sich hin und schreibt Geschichten. Dann kracht Jacky in seine Welt. Ein geheimnisvolles Mädchen aus dem Zirkus. Mit roten Haaren, wasserblauen Augen und keiner Angst vor nichts. Zusammen verbringen sie einen flirrenden, letzten Sommertag, der alles für immer verändert ...</t>
+          <t>Missouri, 1985: Um vor den Problemen zu Hause zu fliehen, nimmt der fünfzehnjährige Sam einen Ferienjob in einem alten Kino an. Und einen magischen Sommer lang ist alles auf den Kopf gestellt. Er findet Freunde, verliebt sich und entdeckt die Geheimnisse seiner Heimatstadt. Zum ersten Mal ist er kein unscheinbarer Außenseiter mehr. Bis etwas passiert, das ihn zwingt, erwachsen zu werden. Eine Hommage an 80's Coming-of-Age-Filme wie 'The Breakfast Club' und 'Stand By Me' - die Geschichte eines Sommers, den man nie mehr vergisst. Ausgezeichnet mit dem Deutschen Jugendliteraturpreis 2022.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>978-3-423-21856-6</t>
+          <t>978-3-257-24674-2</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1825,16 +1905,24 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>DTV</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>detebe</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
@@ -1843,7 +1931,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Breite 122 mm, Höhe 191 mm, Dicke 29 mmGewicht329 g</t>
+          <t>Breite 113 mm, Höhe 180 mm, Dicke 19 mm</t>
         </is>
       </c>
       <c r="P21" t="inlineStr"/>
@@ -1851,28 +1939,34 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Five Survive</t>
+          <t>Provenzalische Täuschung</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>26.90</t>
+          <t>25.90</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Jackson, HollyAgnew, Cherokee MoonÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
+          <t>Bonnet, Sophie</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Eigentlich sollte es ein spaßiger Ausflug werden: Red ist mit fünf Freunden losgefahren, um Spring Break zu feiern. Doch unterwegs bleibt der alte Campingbus liegen - und sie stecken mitten im Nirgendwo fest. Kein Empfang, keine Aussicht auf Hilfe. Und es kommt noch schlimmer, denn draußen im Dunkeln lauert jemand. Sobald sie den Bus verlassen, schießt er auf sie. Seine Behauptung: Jemand aus der Gruppe verheimlicht etwas. Doch wen meint er? Alle sind gezwungen, ihre brisantesten Geheimnisse preiszugeben. Die Spannungen innerhalb des engen Campers steigen. Und nicht alle werden die Nacht überleben ...</t>
+          <t>Aromatische Trüffel, grüne Eichenwälder und ein toter Polizist - ein neuer Fall für den liebeswerten Ermittler Pierre Durand!
+Es ist Trüffelzeit in der Provence. Pierre und Charlotte bereiten ihre Hochzeit vor, als eine Nachricht Sainte-Valérie in Aufregung versetzt: Gilbert Langlois - kürzlich in das Bergdorf gezogen, um Pierre seinen Posten streitig zu machen - liegt tot im Bach. Der Verdacht fällt auf Pierre, doch der glaubt zu wissen, wer der wahre Täter ist: Maurice Marechal, der Bürgermeister des Ortes. Fest entschlossen, ihn des Mordes zu überführen, beginnt Pierre verdeckt zu ermitteln. Die Spur führt ihn nach Mazan unweit des Mont Ventoux, wo sowohl das Opfer als auch Marechal aufgewachsen sind, und zu einem tragischen Fall aus der Vergangenheit. Alles deutet darauf hin, dass beide Geschehnisse miteinander verknüpft sind, als Pierre feststellt, dass es eine Person gibt, die sich an seine Fersen geheftet hat ...
+»Niemand verbindet Genuss und Verbrechen so harmonisch wie Sophie Bonnet in ihren Provence-Krimis.« Hamburger Morgenpost</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>978-3-8466-0182-2</t>
+          <t>978-3-7645-0792-3</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1882,86 +1976,96 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Gebunden</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Lübbe ONE in der Bastei Lübbe AG</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>28.04.2023</t>
+          <t>11.05.2023</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>1. Aufl. 2023</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr"/>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>n-Nr.09</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Breite 145 mm, Höhe 215 mm, Dicke 35 mmGewicht641 g</t>
-        </is>
-      </c>
+      <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ein Lied über der Stadt</t>
+          <t>Victory City</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Arenz, Ewald</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>Rushdie, SalmanRobben, BernhardÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Sommer 1929 in einer Kleinstadt in Franken: Die Pfarrerstochter Luise träumt davon, das Fliegen zu erlernen. Gegen alle Widerstände gelingt es ihr, ihren Traum zu verwirklichen und Pilotin zu werden. Sie verlässt ihre Heimat und wird in München eine gefeierte Kunstpilotin. Als die Nazis an die Macht kommen, muss sie die Fliegerei aufgeben und kehrt nach Franken zurück. Hier ist plötzlich alles anders: Alle schweigen, ganz egal, was passiert. Angst und Misstrauen beherrschen das Miteinander. In der veränderten politischen Lage geraten Louises Familie und auch ihre Jugendliebe Georg mehr und mehr in Gefahr. Ihr Vater, der Terror und Verfolgung anprangert, wird denunziert und von der Gestapo bedroht und Georg als Mitglied des Widerstands gesucht. Schließlich werden Luises Liebe und ihr Können als Pilotin auf eine schwere Probe gestellt.</t>
+          <t>Der neue große Roman über Liebe, Macht und die Kraft des Erzählens von Booker-Preisträger Salman Rushdie
+Südindien im 14. Jahrhundert: Die neunjährige Waise Pampa Kampana wird von einer Göttin auserkoren, ihre menschliche Hülle und ihr Sprachrohr in die Welt zu sein. In ihrem Namen erschafft Pampa aus einer Handvoll Samen eine Stadt: Bisnaga - Victory City, das Wunder der Welt. All ihr Handeln beruht auf der großen Aufgabe, die ihr die Göttin gestellt hat: den Frauen in einer patriarchalen Welt eine gleichberechtigte Rolle zu geben. Aber die Schöpfungsgeschichte Bisnagas nimmt mehr und mehr ihren eigenen Lauf. Während die Jahre vergehen, Herrscher kommen und gehen, Schlachten gewonnen und verloren werden und sich Loyalitäten verschieben, ist das Leben von Pampa Kampana untrennbar mit dieser Stadt verbunden. Von seinem Aufstieg zu einem Weltreich bis zu seinem tragischen Fall.
+Mit »Victory City« kehrt der große Erzähler Salman Rushdie nach Indien zurück, mit einem modernen epischen Roman über Macht, Liebe und darüber, was es bedeutet, ein Mensch zu sein.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>978-3-8321-6669-4</t>
+          <t>978-3-328-60294-1</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Taschenbuch</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Paperback</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>DuMont Buchverlag Gruppe</t>
+          <t>München</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>18.04.2023</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr"/>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
@@ -1971,7 +2075,7 @@
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Breite 125 mm, Höhe 190 mm, Dicke 23 mmGewicht320 gIllustrationenUmschlag mit Strukturkarton, Hochprägung und Lack, Erstmals im Taschenbuch,</t>
+          <t>Breite 147 mm, Höhe 220 mm, Dicke 39 mmGewicht609 g</t>
         </is>
       </c>
       <c r="P23" t="inlineStr"/>
@@ -1979,33 +2083,34 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Twisted Fate, Band 1: Wenn Magie erwacht (Epische Romantasy von SPIEGEL-Bestsellerautorin Bianca Iosivoni | Limitierte Auflage mit Farbschnitt)</t>
+          <t>Der Traum von einem Baum</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>30.90</t>
+          <t>32.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Iosivoni, BiancaLiepins, CarolinUmschlaggestaltung</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>Lunde, MajaAllenstein, UrselÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>___ Limitierte Auflage mit farbigem Buchschnitt! Nur solange der Vorrat reicht! ___
-Als Faith ein Stipendium ergattert, hofft sie vor allem auf eins: ein ganz normales Studium. Doch als sie auf dem Campus auf ein Symbol mit gekreuzten Schwertern und Disteln stößt, ahnt sie, dass ihre Vergangenheit ihr gefolgt ist. Denn plötzlich steht Nate vor ihr, ein Freund aus Kindertagen mit dem gleichen Symbol als Tattoo auf der Haut. Aber auch Jax, der hemmungslos mit Faith flirtet, verbirgt etwas. Was Faith nicht ahnt: Ein längst vergessener Feind hat ihr gemeinsames Schicksal besiegelt.
-Weitere actiongeladene und herzzerreißende Romantasy von Bianca Iosivoni:
-Sturmtochter, Bd. 1-3
-Soul Mates, Bd. 1 &amp; 2
-The Last Goddess, Bd. 1 &amp; 2</t>
+          <t>Das Finale des Klimaquartetts - Großes Maja-Lunde-Porträt auf arte am 10.5. und schon jetzt in der arte Mediathek
+Eine Kammer hoch im Norden, gefüllt mit Pflanzensamen aus aller Welt. Drei Brüder und ihre Großmutter, vereint in der Hoffnung, dieses letzte Band zwischen Mensch und Natur zu behüten.
+Tommy wächst in der kargen Landschaft Spitzbergens mit zwei Brüdern bei seiner geliebten Großmutter auf. Als wichtigste Lebensweisheit gibt sie ihm mit: In einer großflächig zerstörten Welt ist die Saatgutkammer ein Schatz, der mit allen Mitteln beschützt werden muss. Tommy soll diese Aufgabe später von seiner Großmutter übernehmen. In eindrucksvollen Bildern und mit viel Wärme erzählt Maja Lunde von der Bedeutung des Familienzusammenhalts und von unserem Umgang mit der Natur. Sie beschäftigt sich mit den drängenden Fragen unserer Zeit: Wie wurde der Mensch zu einer Spezies, die alles verändert hat? Und sind wir selbst eine bedrohte Art?</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>978-3-473-40219-9</t>
+          <t>978-3-442-75791-6</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2018,20 +2123,20 @@
           <t>Gebunden</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>btb</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>24.04.2023</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>1. Aufl.</t>
-        </is>
-      </c>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>HC - Twisted Fate</t>
+          <t>n-Nr.04</t>
         </is>
       </c>
       <c r="M24" t="inlineStr"/>
@@ -2042,7 +2147,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Breite 154 mm, Höhe 217 mm, Dicke 41 mm</t>
+          <t>Breite 137 mm, Höhe 205 mm, Dicke 46 mm</t>
         </is>
       </c>
       <c r="P24" t="inlineStr"/>
@@ -2050,109 +2155,124 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Eine Nacht, die vor 700 Jahren begann</t>
+          <t>Blutnacht</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>35.00</t>
+          <t>17.90</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+          <t>Enger, ThomasHorst, Jørn LierFrauenlob, GüntherÜbersetzungDörries, MaikeÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Während im Sommer 1944 deutsche Soldaten ungarische Dörfer plündern, stellen sich die Bauern in Kákásd immer noch dieselbe Frage wie vor 700 Jahren: Wie sollen sie leben von dem Lohn, den sie vom Grafen erhalten? Ein Streik könnte alles ändern. Doch in einer Zeit, in der ein Menschenleben billig und Weizen teuer ist, stehen die Chancen auf Erfolg schlecht. Ein junges Liebespaar auf der Flucht und ein Bauer bringen jedoch etwas ins Rollen, und das Leben im Dorf gerät aus den Fugen. Dieser Roman eines der größten ungarischen Romanciers war jahrzehntelang verschollen und erscheint hier zum allerersten Mal.</t>
+          <t>Das dunkelste Kapitel eines Polizisten beginnt dort, wo er nicht hingehört: in einer Gefängniszelle ... Der 4. Fall für Blix &amp; Ramm!
+Alexander Blix, Kriminalhauptkommissar, sitzt in Haft. Eingesperrt mit Dieben, Vergewaltigern und Mördern, die er selbst hinter Gitter gebracht hat, erlebt Blix das dunkelste Kapitel seiner Karriere als Polizist. Doch dann erfährt er, dass außerhalb der Gefängnismauern Lebensgefahr für einen Mithäftling besteht: Ein Killer wartet darauf, dass der Insasse in vier Tagen in die Freiheit entlassen wird - um diesen dann zu ermorden. Nun muss Blix Polizeiarbeit hinter Gittern leisten, ein hochgefährliches Unterfangen, bei dem ihn nur seine Co-Ermittlerin Emma Ramm unterstützen kann ...
+Alle Fälle der norwegischen Bestseller-Serie:
+Blutzahl
+Blutnebel
+Bluttat
+Blutnacht
+Alle Bände unabhängig voneinander lesbar - weitere in Vorbereitung.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>978-3-257-07236-5</t>
+          <t>978-3-7341-1204-1</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Buch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Gebunden</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Diogenes</t>
+          <t>Blanvalet</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>26.04.2023</t>
+          <t>20.04.2023</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>1. A.</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr"/>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>n-Nr.04</t>
+        </is>
+      </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>Breite 116 mm, Höhe 184 mm, Dicke 36 mmGewicht504 g</t>
-        </is>
-      </c>
+      <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Gregs Tagebuch - Schulplaner 2023/2024</t>
+          <t>Babel</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>13.90</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Kinney, Jeff</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
+          <t>Kuang, Rebecca F.Franck, HeideÜbersetzungJordan, AlexandraÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>belletristik scifi_fantasy</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Der Schulplaner für alle Fans von Gregs Tagebuch! Volltreffer! Mit Gregs Schulplaner weißt du immer, wann der nächste Deutschtest ist, wann das Referat in Geschichte ansteht und wann das Training für deine Mannschaft stattfindet. So behältst du stets den Überblick über deine Termine, denn hier ist genug Platz für alle Aufgaben, Notizen und Verabredungen - für jeden Tag und jede Woche. So leicht war es noch nie, einen Plan zu haben - und auch noch nie so lustig!Hier drin findest du:_ Kalendarium von August 2023 bis August 2024_ Ferientermine 2023/2024_ Jahresübersicht 2023/2024_ Notentabelle_ Adressbuch für deine Freunde_ und viele witzige Comics aus den Greg-Büchern</t>
+          <t>»Das Aufregendste im Fantasygenre seit Harry Potter« Denis Scheck1828. Robin Swift, den ein Cholera-Ausbruch im chinesischen Kanton als Waisenjungen zurücklässt, wird von dem geheimnisvollen Professor Lovell nach London gebracht. Dort lernt er jahrelang Latein, Altgriechisch und Chinesisch, um sich auf den Tag vorzubereiten, an dem er in das Königliche Institut für Übersetzung der Universität Oxford - auch bekannt als Babel - aufgenommen werden soll.Oxford ist das Zentrum allen Wissens und Fortschritts in der Welt. Für Robin erfüllt sich ein Traum, an dem Ort zu studieren, der die ganze Macht des britischen Empire verkörpert.Denn in Babel wird nicht nur Übersetzung gelehrt, sondern auch Magie. Das Silberwerk - die Kunst, die in der Übersetzung verloren gegangene Bedeutung mithilfe von verzauberten Silberbarren zu manifestieren - hat die Briten zu unvergleichlichem Einfluss gebracht. Dank dieser besonderen Magie hat das Empire große Teile der Welt kolonisiert.Für Robin ist Oxford eine Utopie, die dem Streben nach Wissen gewidmet ist. Doch Wissen gehorcht Macht, und als chinesischer Junge, der in Großbritannien aufgewachsen ist, erkennt Robin, dass es Verrat an seinem Mutterland bedeutet, Babel zu dienen. Im Laufe seines Studiums gerät Robin zwischen Babel und den zwielichtigen Hermes-Bund, eine Organisation, die die imperiale Expansion stoppen will. Als Großbritannien einen ungerechten Krieg mit China um Silber und Opium führt, muss Robin sich für eine Seite entscheiden ...Aber kann ein Student gegen ein Imperium bestehen?Der spektakuläre Roman der preisgekrönten Autorin Rebecca F. Kuang über die Magie der Sprache, die Gewalt des Kolonialismus und die Opfer des Widerstands.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>978-3-8339-0770-8</t>
+          <t>978-3-8479-0143-3</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Kalender</t>
+          <t>Buch</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Kalender</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Baumhaus Medien</t>
+          <t>Eichborn</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2165,11 +2285,7 @@
           <t>1. Aufl. 2023</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Gregs Tagebuch</t>
-        </is>
-      </c>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr">
         <is>
@@ -2178,7 +2294,7 @@
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Breite 105 mm, Höhe 160 mm, Dicke 13 mm</t>
+          <t>Breite 145 mm, Höhe 215 mm, Dicke 55 mmGewicht915 g</t>
         </is>
       </c>
       <c r="P26" t="inlineStr"/>
@@ -2186,31 +2302,34 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mein Schülerkalender für Potterheads! 2023/2024</t>
+          <t>WWS Pixi-Box 289: Ferien- und Strandgeschichten</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>21.50</t>
+          <t>1.60</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
+          <t>DiverseIllustration:diverse</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>kids bilderbuch</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Magischer Schulalltag garantiert!
-Wo könnte man das neue Schuljahr besser beginnen als an der Schule für Hexerei und Zauberei? Mit dem neuen, magischen Schülerkalender für Potterheads bist du für den Schulalltag bestens gewappnet! Hier findest du alles, was du für die Organisation von Klausurenterminen, Hausaufgaben und Projekten benötigst:
-Praktische Wochen- und Monatsübersichten und Listen erleichtern die OrganisationSpannende Tests, zauberhafte Hacks und leckere Rezepte aus der Schule für Hexerei und ZaubereiMagische Gestaltung und hochwertige Ausstattung mit Glanzfolie und Leseband
-Finde heraus in welches Haus du gehörst, welches Haustier in Hogwarts am besten zu dir passt und teste dein Wissen über die Welt der Hexen und Zauberer! Dank magischen Illustrationen und der hochwertigen Ausstattung mit Leseband und Goldfolie ist er auch optisch ein echter Hingucker!</t>
+          <t>Der Sommer kann kommen! Denn jetzt geht es mit Pixi in die Ferien und an den Strand. Dabei fällt auf, dass sich am Strand nicht nur Meerestiere tummeln, sondern auch Piraten ... und wie schön es sein kann, einfach mal im Garten zu sein. Mit diesen acht Pixi-Geschichten wird es nirgendwo langweilig, weder auf Reisen noch zu Hause!
+In der Pixi-Serie "Ferien- und Strandgeschichten" sind folgende Bücher enthalten:
+Jule und Rosetta am StrandEnrico und die faulen PiratenNachts ist alles andersFiete, der StrandpiratDer Schatz am StrandFerien im GartenKäpt'n Schiefzahn und das GlückchenAufregung am Baggersee</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>978-3-7459-1568-6</t>
+          <t>978-3-551-03918-7</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2220,17 +2339,17 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Gebunden</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Edition Michael Fischer</t>
+          <t>Carlsen</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>19.04.2023</t>
+          <t>27.04.2023</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
@@ -2238,45 +2357,45 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
-          <t>Deutsch</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>Breite 153 mm, Höhe 216 mm, Dicke 20 mmGewicht510 g</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr"/>
+          <t>DeutschGewicht19 gIllustrationenFarbig illustriert</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>55688599</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Liar - Tödlicher Verrat</t>
+          <t>1941. Liebe in herzlosen Zeiten</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>22.50</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Jackson, LisaLake-Zapp, KristinaÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
+          <t>Cantieni, Margrit</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>taschenbuch schweizer</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Eine skandalumwitterte Familie, eine verhängnisvolle Affäre und ein mörderischer Plan:
-Bestseller-Autorin Lisa Jackson begeistert mit einem dramatischen Thriller voller unvorhersehbarer Wendungen.
-Nach einem bösen Streit mit ihrem schwerreichen, notorisch untreuen Freund James Cahill will Megan Travers nur noch weg von dessen Ranch in den Cascade Mountains. Trotz eines heftigen Schneesturms macht sie sich auf den Weg zu ihrer Schwester, doch dort kommt sie nie an. Als die Detectives Brett Rivers und Wynonna Mendoza James befragen wollen, finden sie ihn mit einer Kopfverletzung im Krankenhaus vor. James sagt aus, er könne sich an nichts erinnern, weder an Megan noch an seine zahlreichen Affären. Kurz darauf bringen die Morde an zwei Frauen aus seinem Umfeld den Herzensbrecher in Erklärungsnöte ...
-Hochspannung, eine Prise Romantik, jede Menge zwischenmenschliche Verwicklungen und kaltblütige Morde - all das bietet dieser Thriller von Bestseller-Autorin Lisa Jackson. Liar - Tödlicher Verrat ist unabhängig lesbar.
-Entdecken Sie auch die anderen Thriller von Lisa Jackson, z.B. Showdown - Ich bin dein Tod um zwei Schwestern, die erbitterte Rivalinnen sind, oder Paranoid, worin es um späte Rache in einer ehemaligen Highschool-Clique geht.</t>
+          <t>Gegen jeden WiderstandSommer 1941. Tausende polnische Soldaten werden auf der Flucht vor der deutschen Wehrmacht in der Schweiz interniert und von den Einheimischen als Helden gefeiert. Doch bald schon kippt die Stimmung, und die zuvor willkommenen Flüchtlinge werden zur vermeintlichen Bedrohung. So auch Marek, der im Arbeitslager auf die junge Sofia trifft. Es ist Liebe auf den ersten Blick, aber je länger der Krieg dauert, desto unerwünschter wird ihre Beziehung. Schaffen sie es, sich den Regeln der Gesellschaft zu widersetzen und ihr gemeinsames Glück zu finden?</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>978-3-426-52652-1</t>
+          <t>978-3-7408-1786-2</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2289,22 +2408,14 @@
           <t>Paperback</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Droemer/Knaur</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>02.05.2023</t>
+          <t>25.04.2023</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Ein San-Francisco-Thriller</t>
-        </is>
-      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr">
         <is>
@@ -2313,38 +2424,57 @@
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Breite 125 mm, Höhe 190 mm, Dicke 34 mm</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr"/>
+          <t>Breite 135 mm, Höhe 205 mm, Dicke 25 mmGewicht320 g</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>55652604</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Strandhaus Meeresrauschen</t>
+          <t>Hochzeitsglocken auf der kleinen Insel</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>17.90</t>
+          <t>19.90</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Säfstrand, CarolineWerner, StefanieÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
+          <t>Colgan, JennyHagemann, SonjaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Der Klang der Wellen, der Geruch des Meeres und ein Haus voller Bücher - der neue Roman von Schwedens Feel-Good-Königin Caroline Säfstrand!
-Die Autorin Inez lebt zurückgezogen in einem kleinen Strandhaus an der schwedischen Küste, sie umgibt sich lieber mit Büchern als mit Menschen. Als ihre Nachbarin stirbt, beschließt sie, mit ihrem Leben aufzuräumen: Sie möchte vorsorgen, ihr Haus ausmisten und ihr letztes, alles offenbarendes Buch schreiben. Als Inez kurz darauf stürzt, ist sie gezwungen, das Dienstmädchen Meja einzustellen. Sie soll ihr beim Entrümpeln des Strandhauses helfen. Die einzige Regel: Unter keinen Umständen darf der blaue Ordner mit dem Buchskript geöffnet werden! Doch natürlich sieht Meja die geheimen Worte eines Tages ... Das Treffen zwischen Inez, die im hohen Alter mit ihrer Vergangenheit versöhnt werden muss, und der hoffnungslosen Meja, die nach einer Zukunft sucht, hat für die beiden ungleichen Frauen unvorhergesehene Folgen ...
-Lust auf noch mehr schwedische Wohlfühllektüre? Dann lesen Sie auch »Strandhotel Meeresbrise« von Caroline Säfstrand.</t>
+          <t>Inselflair und Glücksgefühle: Mit »Hochzeitsglocken auf der kleinen Insel« führt SPIEGEL-Bestsellerautorin Jenny Colgan ihre Frauenroman-Reihe um die kleine Sommerküche zum krönenden Abschluss.
+»Wohlfühlfaktor: Sehr hoch, wie immer bei Jenny Colgan, der Meisterin der Romane, in die man gleich einziehen will, weil ihre Welten sich so kuschelig anfühlen beim Lesen.« Berner Zeitung
+Gleich drei verliebte Paare suchen in »Hochzeitsglocken auf der kleinen Insel« nach ihrem Happy end - Romantik und Sommersonne garantiert!
+Instagram-Star Olivia plant eine Hochzeit, die alle anderen in den Schatten stellen soll. Und das ausgerechnet auf der schottischen Insel Mure. Das Event wäre die Werbung, die Hotel-Chefin Flora braucht, um das brandneue Hotel »The Rock« ans Laufen zu bringen. Dumm nur, dass Olivias extravagante Ideen Floras eigene Pläne durcheinanderwirbeln.
+Denn Flora möchte mit »ihrem« Joel auch endlich den Bund fürs Leben schließen. Doch die beiden haben ziemlich unterschiedliche Vorstellung vom perfekten Fest - er: so klein wie möglich, sie: am liebsten mit der ganzen Welt -, und jetzt funkt auch noch Olivia dazwischen.
+Lorna, die Leiterin der Inselschule, macht sich ebenfalls Gedanken über die Zukunft. Sie und Saif, der syrische Arzt, leben ihre Liebe weiterhin nur im Verborgenen. Werden Sie irgendwann ganz offen ein Paar sein dürfen?
+Love is in the air auf der kleinen Insel Mure! Werden die Hochzeitsglocken in diesem Sommer gleich für drei Paare läuten?
+Glücksgefühle in Buchform - die Reihe um "Floras Küche" von SPIEGEL-Bestsellerautorin Jenny Colgan
+Band 1: Die kleine Sommerküche am Meer
+Band 2: Hochzeit in der kleinen Sommerküche am Meer
+Band 3: Weihnachten in der kleinen Sommerküche am Meer
+Band 4: Weihnachten im kleinen Inselhotel
+Band 5: Hochzeitsglocken auf der kleinen Insel
+Und exklusiv im e-book die Novella: Begegnung in der kleinen Sommerküche am Meer</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>978-3-7341-1241-6</t>
+          <t>978-3-492-31910-2</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2359,61 +2489,59 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Blanvalet</t>
+          <t>Piper</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>20.04.2023</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Deutsche Erstausgabe</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr"/>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>n-Nr.05</t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr">
         <is>
           <t>Deutsch</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>Breite 119 mm, Höhe 188 mm, Dicke 34 mmGewicht353 g</t>
-        </is>
-      </c>
+      <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Good Places for Good People</t>
+          <t>Wo wir uns trafen</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>35.90</t>
+          <t>32.90</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Diallo, FranziskaHehl, Judith</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
+          <t>Lundberg, SofiaDörries, MaikeÜbersetzungSchöps, KerstinÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Dorthin reisen, wo Nachhaltigkeit gelebt wird
-Nachhaltigkeit wird inzwischen genauso selbstverständlich erwartet wie einmalige Erlebnisse und Erholung. Der Inspirations-Bildband Good Places for Good People präsentiert 50 Unterkünfte und Destinationen in Europa, die den aktuellen Umweltstandards nicht nur gerecht werden, sondern auch in jeder Preiskategorie für eine genuss- und stilvolle Auszeit sorgen.
-Ob Stadthotel oder Baumhaus, Wellness-Resort oder Bauernhof: Die Gastgeber:innen dieser handverlesenen Orte setzen sich für einen schonenden Umgang mit Ressourcen ein, kochen frisch und regional und engagieren sich für Natur und Menschen in ihrer Region. Die perfekte Inspiration für alle, die umweltbewusst reisen wollen - ohne Kompromisse.
-Wirklich nachhaltige Reiseideen für ein gutes Urlaubsgefühl</t>
+          <t>Nur wahre Freundschaft berührt dein Herz ...
+Lidingö, Südschweden: Jeden zweiten Samstag sitzt die frisch geschiedene Esther auf einer Bank unter einer alten Eiche und schaut hinaus aufs Meer. Die Wochenenden, die ihr Sohn bei seinem Vater verbringt, sind schwer, und hier kann Esther ihren Gefühlen freien Lauf lassen. Eines Tages trifft sie dort auf Rut, eine alleinstehende, ältere Dame, die Esther mit ihrer warmherzigen Art tröstet. Zwischen den beiden Frauen entsteht eine tiefe Freundschaft, und die Bank am Meer wird zu ihrem regelmäßigen Treffpunkt. Doch dann verschwindet Rut, und als Esther sich auf die Suche nach ihr macht, kommt sie einer dramatischen Lebensgeschichte auf die Spur ...</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>978-3-95889-449-5</t>
+          <t>978-3-442-31645-8</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2423,16 +2551,24 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Paperback</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Goldmann</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>08.05.2023</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
@@ -2442,7 +2578,7 @@
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Breite 170 mm, Höhe 240 mm, Dicke 20 mmGewicht734 g</t>
+          <t>Breite 148 mm, Höhe 221 mm, Dicke 37 mmGewicht564 g</t>
         </is>
       </c>
       <c r="P30" t="inlineStr"/>
@@ -2450,28 +2586,33 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Alle Mamas</t>
+          <t>Wo wir uns trafen</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>23.90</t>
+          <t>32.90</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ellis, Sarah KateEllis-Henderson, KristenRambaldi, MaxIllustrationenFiedler-Tresp, SonjaÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
+          <t>Lundberg, SofiaDörries, MaikeÜbersetzungSchöps, KerstinÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>»Alle Mamas« ist Liebesbrief und Lobeshymne an alle Mütter in einem. Die Botschaft ist: Alle Mütter zu feiern, weil sie unglaubliches leisten. Ob Pilotin, Ärztin, alleinerziehend, in Form zweier Väter oder als tolle Oma - alle Mütter zeichnen sich vor allem durch ihre Fürsorge und Liebe für ihre Kinder aus. Die zeitgemäßen, farbenfrohen Illustrationen stecken voller Leben und zeigen wie vielseitig Familien heute sind.</t>
+          <t>Nur wahre Freundschaft berührt dein Herz ...
+Lidingö, Südschweden: Jeden zweiten Samstag sitzt die frisch geschiedene Esther auf einer Bank unter einer alten Eiche und schaut hinaus aufs Meer. Die Wochenenden, die ihr Sohn bei seinem Vater verbringt, sind schwer, und hier kann Esther ihren Gefühlen freien Lauf lassen. Eines Tages trifft sie dort auf Rut, eine alleinstehende, ältere Dame, die Esther mit ihrer warmherzigen Art tröstet. Zwischen den beiden Frauen entsteht eine tiefe Freundschaft, und die Bank am Meer wird zu ihrem regelmäßigen Treffpunkt. Doch dann verschwindet Rut, und als Esther sich auf die Suche nach ihr macht, kommt sie einer dramatischen Lebensgeschichte auf die Spur ...</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>978-3-96846-113-7</t>
+          <t>978-3-442-31645-8</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2481,20 +2622,24 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>GebundenFormatBilderbuch</t>
+          <t>Gebunden</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Migo</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>14.04.2023</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr"/>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr">
@@ -2504,7 +2649,7 @@
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Breite 224 mm, Höhe 287 mm, Dicke 9 mmGewicht368 g</t>
+          <t>Breite 148 mm, Höhe 221 mm, Dicke 37 mmGewicht564 g</t>
         </is>
       </c>
       <c r="P31" t="inlineStr"/>
@@ -2512,30 +2657,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Star Switch â Mein (Dein) Leben steht Kopf</t>
+          <t>Going Zero</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23.90</t>
+          <t>34.00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Dixon, AleshaBirchall, KatyKilchling, VerenaÜbersetzung</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Ich bin du, und du bist ich
-Naomi ist dreizehn und der größte Popstar der Welt. Sie tritt in Amerika auf, tourt durch Japan, und alle, einfach alle finden sie toll. Aber richtige Freunde hat sie keine, und wenn sie mal shoppen gehen will, wird das Einkaufszentrum nur für sie geöffnet - nachts, wenn sonst niemand dort ist. Ruby ist Naomis größter Fan. Sie kennt die Texte zu jedem ihrer Lieder, sie kann alle Moves nachmachen und träumt heimlich davon, Naomis allerbeste Freundin zu sein. Als die beiden Mädchen zufällig aufeinandertreffen und - zack! - die Körper tauschen, gerät Ruby von einer Sekunde auf die nächste ins Rampenlicht. Wird sie ihr neues Superstar-Leben lieben oder wird sie am Ende genauso einsam sein wie Naomi? Und wird Naomi herausfinden, dass sie weltberühmt und doch ein normales Mädchen sein kann?
-Erfolgreiches Dream-Team: Die Bestsellerautorin Katy Birchall (»Emma Charming«) und der Show-Star Alesha Dixon (»Britan's Got Talent«) schreiben zusammen eine Körpertauschgeschichte voller Drehungen und Wendungen, bei der man nie weiß, was als Nächstes kommt - witzig, turbulent und charmant!</t>
+          <t>Hat man als Einzelner überhaupt eine Chance gegen das System? Eine junge Bibliothekarin aus Boston ist entschlossen, es zu versuchen - ihr bleibt keine Wahl. Und so greift sie zu, als sich die Einladung zu einem ungewöhnlichen Kräftemessen bietet: dem Betatest von FUSION, einem Projekt der US-Geheimdienste und des Social-Media-Moguls Cy Baxter. Wem es gelingt, 30 Tage unauffindbar zu bleiben, dem winken 3 Millionen Dollar. Doch Kaitlyn geht es um etwas anderes.</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>978-3-7373-4270-4</t>
+          <t>978-3-257-07192-4</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2550,7 +2697,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>FISCHER KJB</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2558,7 +2705,11 @@
           <t>26.04.2023</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr">
@@ -2568,7 +2719,7 @@
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Breite 148 mm, Höhe 219 mm, Dicke 29 mmGewicht481 g</t>
+          <t>Breite 116 mm, Höhe 184 mm, Dicke 30 mmGewicht403 g</t>
         </is>
       </c>
       <c r="P32" t="inlineStr"/>
@@ -2576,47 +2727,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Die Robot-Kids 1: Rettung von Moto-5</t>
+          <t>Going Zero</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>13.90</t>
+          <t>34.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Flessner, BerndFlessner, HannahGrubing, TimoIllustrationen</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Modernes Erstlesebuch mit den Robot-Kids
-In den Ferien besuchen Alex, Milo, Lea und deren Schwester Sam ein Forschungsinstitut. Alex' Tante Jana ist Roboter-Expertin und sie testet und entwickelt dort verschiedene Modelle. Die Kinder sind sofort Feuer und Flamme, als sie dort den ausrangierten Serviceroboter Moto-5 entdecken. Mit viel Köpfchen und Kreativität machen sie sich ans Werk. Denn wenn sie es schaffen, den Roboter wieder zum Laufen zu bringen, dürfen sie Moto-5 behalten!
-Ein spannendes Erstlese-Abenteuer, das Lust aufs Lesen macht.
-Kurze Kapitel, eingängiger Text, coole Illustrationen sowie eine Lese-Urkunde zur Belohnung motivieren zum Weiterlesen.
-Der Auftakt zur neuen Reihe "Die Robot-Kids" vom Bestseller-Duo Bernd und Hannah Flessner, mit tollen Bildern von Timo Grubing!
-Mit viel Witz, coolen Illustrationen und Leseurkunde gelingt es dem Autorenduo Flessner, ein wichtiges Zukunfsthema kindgerecht und spannend aufzuarbeiten.
-Am Ende erklärt der Roboter "Moto-5" in einem kleinen Wörterbuch die Fachbegriffe zusätzlich.
-------------------------------
-Die Robot-Kids, das sind: Alex, Milo, Lea und deren kleine Schwester Sam. Alex' Tante Jana ist Roboter-Expertin und häufig dürfen die Kinder sie in ihrem Forschungslabor besuchen. Dort gibt es viele unterschiedliche Roboter zu sehen, die verschiedenene Aufgaben zu erfüllen haben. Fast alle dienen dazu. Menschen in Situationen zu helfen und oft auch ihr Leben zu schützen, wie zum Beispiel die wie große Käfer aussehenden Löschroboter.
-Die Kinder dürfen auch beim Testen der Roboter zuschauen, und dabei geschehen immer wieder unvorhergesehene Dinge, die lustig, aber auch gefährlich sein können.
-Für viel Spaß sorgt auch Janas Mann Markus, der Erfinder ist und ebenfalls mit Robotern experimentiert. Seine Arbeit an einer Nudelmaschine ist auf jeden Fall noch verbesserungswürdig ...
-------------------------------
-In Band 1 "Rettung von Moto-5" (ISBN 978-3551690203) reparieren die Kinder den Service-Roboter Moto-5 und bewahren ihn so vor dem Verschrotten.
-In Band 2 "Die Löschroboter" (ISBN 978-3551690210, erscheint im Juli 2023) testen die Kinder Löschroboter bei einem vorgetäuschten Waldbrand und kommen dabei ganz schön ins Schwitzen.
-In Band 3 (erscheint im Juli 2024) werden die Kinder Robot-Kids ein Abenteuer in den Bergen erleben.
-Und alle, die weitere Abenteuer mit den Robot-Kids erleben wollen, dürfen sich freuen, denn es sind auch Abenteuer für fortgeschrittene Leser_innen geplant!
-------------------------------
-Einfach Lesen lernen:
-2. Lesestufe: Kurze Sätze, große SchriftKleine Texteinheiten in Kombination mit vielen bunten BildernComicelemente, um die Sehgewohnheiten von Kindern zu berücksichtigen
-Spannung, Abenteuer, Technik - packender Mix für Leseanfänger_innen ab 6Mit Lese-Urkunde und kleinem Wörterbuch zu Fachbegriffen</t>
+          <t>Hat man als Einzelner überhaupt eine Chance gegen das System? Eine junge Bibliothekarin aus Boston ist entschlossen, es zu versuchen - ihr bleibt keine Wahl. Und so greift sie zu, als sich die Einladung zu einem ungewöhnlichen Kräftemessen bietet: dem Betatest von FUSION, einem Projekt der US-Geheimdienste und des Social-Media-Moguls Cy Baxter. Wem es gelingt, 30 Tage unauffindbar zu bleiben, dem winken 3 Millionen Dollar. Doch Kaitlyn geht es um etwas anderes.</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>978-3-551-69020-3</t>
+          <t>978-3-257-07192-4</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2631,20 +2767,20 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Carlsen</t>
+          <t>Diogenes</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>27.04.2023</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>n-Nr.01</t>
-        </is>
-      </c>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr">
         <is>
@@ -2653,7 +2789,7 @@
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Breite 160 mm, Höhe 215 mm, Dicke 12 mm</t>
+          <t>Breite 116 mm, Höhe 184 mm, Dicke 30 mmGewicht403 g</t>
         </is>
       </c>
       <c r="P33" t="inlineStr"/>
@@ -2661,51 +2797,60 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Warum wir nicht durch Wände gehen*</t>
+          <t>Sommernächte in Paris</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>36.90</t>
+          <t>16.90</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Aigner, Florian</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
+          <t>Swan, KarenWittich, GertrudÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Die Welt der Quanten ist voller atemberaubender Geschichten und Ideen - von winzigen Teilchen, die sich an zwei verschiedenen Orten gleichzeitig befinden, von Katzen, die gleichzeitig lebendig und tot sind, von geheimnisvoller Teleportation. Gleichzeitig bestimmt Quantenphysik längst unseren Alltag: Laser, Mikrochips oder MRT-Bilder wären ohne Quantentheorie nicht möglich. Immer wieder heißt es: Quanten sind so kompliziert, dass sie höchstens von ein paar Wissenschaftsgenies verstanden werden können. Stimmt nicht, beweist Wissenschaftserklärer und Quantenphysiker Florian Aigner in seinem neuen Buch! Die Welt der Quanten kann jeder verstehen, wenn wir aus unseren gewohnten Denkmustern ausbrechen. Wie das gelingt, zeigt der Bestsellerautor auf einem Trip in die erstaunliche Welt der kleinsten Teilchen - unterhaltsam, höchst erhellend und horizonterweiternd.</t>
+          <t>Ein unvergesslicher Sommer in der Stadt der Liebe ...
+Die Kunstagentin Flora Sykes ist ständig in der Welt unterwegs. Für ein Privatleben oder eine ernsthafte Beziehung bleibt da keine Zeit. Nun führt sie ein geheimnisvoller Auftrag nach Paris, wo die wohlhabende Familie Vermeil ein Apartment voller Kunstschätze geerbt hat, das seit über siebzig Jahren niemand mehr betreten hat. Warum war es so lange verschlossen? Und woher stammen die Bilder? Statt Antworten zu finden, stößt Flora bei ihren Nachforschungen auf immer mehr Geheimnisse. Und zu allem Überfluss lenkt Xavier Vermeil, der unverschämt gut aussehende Sohn der Erben, sie immer wieder von der Arbeit ab ...</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>978-3-7106-0689-2</t>
+          <t>978-3-442-49396-8</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Buch</t>
+          <t>Taschenbuch</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Gebunden</t>
+          <t>Paperback</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Brandstätter</t>
+          <t>Goldmann</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>24.04.2023</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr"/>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr">
@@ -2715,7 +2860,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Breite 142 mm, Höhe 218 mm, Dicke 27 mmGewicht558 g</t>
+          <t>Breite 126 mm, Höhe 187 mm, Dicke 35 mmGewicht394 g</t>
         </is>
       </c>
       <c r="P34" t="inlineStr"/>
@@ -2723,7 +2868,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Peppino</t>
+          <t>One of the Girls</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2733,18 +2878,23 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Ziegler, UrsinaJucker, SitaIllustrationen</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
+          <t>Clarke, LucyHofstetter, UrbanÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Peppinos Vater Peppone ist Schausteller. Als dieser sich verletzt, ist Peppino plötzlich auf sich allein gestellt. Er meistert diese Herausforderung bravourös, denn wie sich herausstellt, steckt im kleinen Peppino ein großer Künstler, der die Menschen mit seinen Bildern begeistert. » Peppino « erzählt die zeitlose Geschichte eines Jungen, der sich in schwierigsten Umständen behauptet. Das Buch erschien erstmals 1971 und transportiert den Geist seiner Zeit. Jetzt geben wir den Schweizer Bilderbuch-Klassiker in einer sorgfältig gestalteten Ausgabe neu heraus.</t>
+          <t>Sechs Frauen. Sechs Geheimnisse. Eine Leiche.
+Es sollte der perfekte Kurzurlaub werden: Lexi reist mit fünf Freundinnen auf eine griechische Insel, um ihren Junggesellinnenabschied zu feiern. Von der abgelegenen Villa mit Meerblick bis hin zu den malerischen Tavernen und weiß getünchten Straßen scheint der Urlaub zu schön, um wahr zu sein. Und tatsächlich bekommt die Idylle bald Risse, denn abgesehen von ihrer Freundschaft mit Lexi haben die Frauen nur eines gemeinsam: Sie alle haben etwas zu verbergen. Nach und nach kommen versteckte Absichten ans Licht, Geheimnisse werden enthüllt und die Masken fallen - bis eine Leiche auf den Klippen unterhalb der Villa liegt...</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>978-3-314-10640-8</t>
+          <t>978-3-423-26359-7</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2754,10 +2904,14 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Gebunden</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr"/>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>DTV</t>
+        </is>
+      </c>
       <c r="J35" t="inlineStr">
         <is>
           <t>20.04.2023</t>
@@ -2773,7 +2927,7 @@
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Breite 280 mm, Höhe 215 mm, Dicke 15 mmGewicht402 gIllustrationenDurchgehend farbig illustriert</t>
+          <t>Breite 136 mm, Höhe 210 mm, Dicke 31 mmGewicht450 g</t>
         </is>
       </c>
       <c r="P35" t="inlineStr"/>
@@ -2781,30 +2935,33 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Unkaputtbar: Mein erstes Wimmelbuch: Wir machen einen Ausflug</t>
+          <t>Die Tage in der Buchhandlung Morisaki</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8.90</t>
+          <t>26.90</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Schumann, SibylleReckers, SandraIllustrationen</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+          <t>Yagisawa, SatoshiEnders, UteÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Die unkaputtbaren Wimmelbücher, die alles mitmachen
-Komm, wir machen einen Ausflug: Was können wir im Wald alles entdecken? Wen triffst du im Tierpark? Und wo hat sich eigentlich der kleine Teddy versteckt? Ein erstes Wimmelbuch zum Suchen, Finden und Weitererzählen.
-Für alle Baby-Pixi-Fans: Die neue Wimmelbuchreihe kombiniert spannende Themen mit dem beliebten unkaputtbaren Material. Genau so leicht, handlich und robust wie die bekannten Baby Pixis - aber größer, umfangreicher und ideal für Kinder ab 2 Jahren. Die unkaputtbaren Wimmelbücher, die alles mitmachen!</t>
+          <t>Die 25-jährige Takako hat einen Job, eine Wohnung in Tokio und einen festen Freund. Als dieser ihr eines Abends freudig eröffnet, er werde heiraten - und zwar eine andere -, fällt sie aus allen Wolken. Vor Kummer verkriecht sie sich und kündigt ihren Job. Als ihr Onkel ihr anbietet, eine Zeitlang in seinem Antiquariat im berühmten »Bücherviertel« Tokios, Jimb ch , auszuhelfen und dort auch unterzukommen, findet sie das zwar zunächst alles andere als reizvoll, willigt aber ein. Doch in dem kleinen Zimmer über dem Laden, inmitten von Büchern, entdeckt sie ihre Leidenschaft fürs Lesen - und schöpft allmählich wieder neue Kraft.
+Satoshi Yagisawa erzählt in seinem Bestseller schnörkellos, leichtfüßig und charmant von einer jungen Frau, die durch die heilsame Kraft des Lesens zurück ins Leben und zu neuen Freundschaften findet.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>978-3-551-06254-3</t>
+          <t>978-3-458-64369-2</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2814,25 +2971,17 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Paperback</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Carlsen</t>
-        </is>
-      </c>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
-          <t>27.04.2023</t>
+          <t>17.04.2023</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>Unkaputtbar</t>
-        </is>
-      </c>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
@@ -2841,10 +2990,1225 @@
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Breite 145 mm, Höhe 170 mm, Dicke 4 mmGewicht30 g</t>
-        </is>
-      </c>
-      <c r="P36" t="inlineStr"/>
+          <t>Breite 132 mm, Höhe 214 mm, Dicke 28 mmGewicht340 g</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>55184394</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Das Leben ist ein vorübergehender Zustand</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>20.90</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>taschenbuch biografien</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>«Ein erschütterndes Buch, aber es ist eine heilsame, eine befreiende Erschütterung, eine hilfreiche, mit der man deutlich weiter kommt als mit aller wohltuenden Erträglichkeit. [...] im Kern eine Liebesgeschichte - und ein großes Zeugnis.» Sten Nadolny
+Ein Schlaganfall, zehn Tage später der zweite, haben ihren Mann aus allem herauskatapultiert, was er bis dahin gelebt hatte. Und aus ihr wird die Frau des Kranken. Wie liebt und hütet man einen Mann, der an dem Tag zusammenbricht, an dem man ihm gesagt hat, man könne nicht mehr leben mit ihm? Wie schafft man die Balance, in der Krankheit zu sein und im Leben zu bleiben? Gabriele von Arnim beschreibt in diesem literarischen Text, wie schmal der Grat ist zwischen Fürsorge und Übergriffigkeit, Zuwendung und Herrschsucht. Wie leicht Rettungsversuche in demütigender Herabwürdigung enden. Und Aufopferung erbarmungslos wird.
+«Das Leben ist ein vorübergehender Zustand» ist eine leidenschaftliche, so kühle wie zärtliche Erzählung eines bedrängten Lebens.
+«Bitte lesen Sie dieses Buch, das mit einer solch stillen Wucht daherkommt, dass man zunächst gar nicht merkt, wie es einen umhaut. Ganz große Kunst und so nah am Leben.» Daniel Schreiber</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>978-3-499-00634-0</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Rowohlt TB.</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>18.04.2023</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Breite 125 mm, Höhe 190 mm, Dicke 18 mmGewicht213 g</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Das Ferienhaus - Und du denkst, du bist sicher</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Ewan, C.M.Stratthaus, BerndÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Eine Familie. Ein abgelegenes Haus. Und es gibt kein Entkommen ...
+Als Tom Sullivan nachts um zwei ein Fenster zerbrechen hört, werden seine schlimmsten Albträume Wirklichkeit: Jemand ist ins Haus eingedrungen und trachtet ihm und seiner Familie nach dem Leben. Sein Feriendomizil mitten im schottischen Nirgendwo, das eigentlich für ein paar Wochen zu einem beschaulichen Urlaubsort werden sollte, wird zur tödlichen Falle. Ein atemberaubendes Versteckspiel beginnt, während dem sich Tom mehr als einmal fragt, ob er denen, die ihm am nächsten sind, wirklich vertrauen kann. Sogar seine Ehefrau Rachel scheint irgendetwas vor ihm zu verbergen ...
+Freuen Sie sich auf noch mehr nervenzerreißende Spannung von C.M. Ewan - sein neuer Thriller »Etage 13« ist ab Frühjahr 23 bei Blanvalet erhältlich!</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>978-3-7341-1243-0</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Blanvalet</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Erstmals im TB</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Breite 127 mm, Höhe 188 mm, Dicke 38 mmGewicht420 g</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wenn jeder dich mag, nimmt keiner dich ernst</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Wehrle, Martin</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>fachbuecher psychologie psychologie</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Sagen Sie zu selten, was Sie wirklich wollen?
+Wie oft sagen Sie, was tatsächlich in Ihnen vorgeht? Und wie oft behalten Sie Ihre Meinung für sich, aus Sorge, anderen damit auf den Schlips zu treten? Wer alles tut, was andere von ihm wollen, ist zwar beliebt - aber lediglich als leichtes Opfer. Nur wem es gelingt, sich nicht verunsichern zu lassen und auch unbequeme Haltungen zu vertreten, wird die eigenen Ziele erreichen. Bestseller-Autor Martin Wehrle zeigt, wie Sie in jeder Lebenslage Ihre Selbstachtung verteidigen.
+Für alle, die
+_ sich nicht länger ausnutzen lassen wollen,
+_ ihren Willen durchsetzen möchten,
+_ souverän kontern wollen, wenn ihr Gegenüber sie überfordert, kleinmacht oder angreift.
+Ein Buch voller Kraft und Inspiration, das Sie selbstbewusster und schlagfertiger macht!</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>978-3-442-39409-8</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Mosaik</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Breite 139 mm, Höhe 207 mm, Dicke 31 mmGewicht421 g</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Wenn sie wüsste</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>McFadden, FreidaGravert, AstridÜbersetzungWeitbrecht, RenateÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Wenn du glaubst, diese Geschichte zu durchschauen, fängt sie erst an
+Mit farbig gestaltetem Buchschnitt nur in limitierter Erstauflage (Lieferung je nach Verfügbarkeit)
+Millie kann ihr Glück kaum fassen, als die elegante Nina ihr die Stelle als Haushaltshilfe inklusive Kost und Logis bei ihrer Familie auf Long Island anbietet. Schließlich hat sie eine Vergangenheit, von der niemand etwas wissen soll. Doch kaum ist Millie eingezogen, zeigt Nina ihr wahres Gesicht: Sie verwüstet das Haus und unterstellt ihr Dinge, die sie nicht getan hat. Ihre verwöhnte Tochter behandelt Millie ohne jeden Respekt. Nur Ninas attraktiver Mann Andrew ist nett zu ihr. Wäre da nur nicht Ninas wachsende Eifersucht. Hat sie Millie nur eingestellt, um ihr das Leben zur Hölle zu machen? Oder hat auch sie ein dunkles Geheimnis, von dem niemand etwas erfahren darf?</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>978-3-453-47190-0</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Heyne</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>11.05.2023</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Deutsche Erstausgabe</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 207 mm, Dicke 34 mmGewicht474 g</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Die Moskau-Connection</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Bingener, ReinhardWehner, Markus</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>fachbuecher geschichte politik</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>DER PIPELINE-DEAL: HINTER DEN KULISSEN EINES VERHÄNGNISVOLLEN NETZWERKS
+Deutschland hat über viele Jahre die Gefahr ignoriert, die von Putins Regime ausging. Es hat die Warnungen seiner europäischen Nachbarn in den Wind geschlagen und sich von Gas und Öl aus Russland immer abhängiger gemacht. Die Folge ist eine schwere Wirtschaftskrise, die den Wohlstand der Bundesrepublik langfristig schmälern wird.
+Wie konnte es dazu kommen? Welche Rolle spielte dabei Gerhard Schröder als SPD-Bundeskanzler und späterer Gas-Lobbyist mit seinem weitverzweigten Netz in Politik und Wirtschaft? Warum schlug CDU-Kanzlerin Angela Merkel keinen weitsichtigeren Kurs ein? Welche geschäftlichen und politischen Verbindungen, aber auch welche wirtschaftlichen und strategischen Interessen führten dazu, dass Deutschland auf Putin setzte, obwohl er schon vor seinem Überfall auf die Ukraine Kriege geführt, die Opposition ausgeschaltet und Freiheits- und Menschenrechte missachtet hatte? Die FAZ-Korrespondenten Reinhard Bingener und Markus Wehner decken die Moskau-Connection der deutschen Politik auf und zeigen, wie eine der größten Fehleinschätzungen deutscher Außenpolitik seit 1945 möglich wurde.
+Hannover - Berlin - Moskau: Die große Recherche über Gerhard Schröders verhängnisvolles Netzwerk in Politik und Wirtschaft Wie zwielichtige Honorarkonsuln, ominöse Bauunternehmer, Ex-Stasi-Majore und naive Entspannungspolitiker Deutschland in die Abhängigkeit vom Kreml geführt haben Für Leser:innen von Catherine Belton "Putins Netz"</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>978-3-406-79941-9</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Beck</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>02.05.2023</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>4. A.</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Breite 124 mm, Höhe 205 mm, Dicke 18 mmGewicht330 g</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Am Horizont wartet die Sonne</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Werkmeister, Meike</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Der große neue Sommerroman der SPIEGEL-Bestsellerautorin
+Es gibt keine Zufälle, es gibt nur Zeichen. Davon ist die Hamburger Autorin Katrin überzeugt. Doch während sie Bücher schreibt, die anderen Orientierung geben sollen, steckt sie selbst in einer Lebenskrise. Bis das Schicksal auch ihr ein Zeichen gibt: Als sie einen Liebesbrief findet, adressiert an einen Filipe in Portugal, beschließt sie, dem Empfänger die Botschaft persönlich zu überbringen. Mit ihrer Freundin Julia reist sie auf eine idyllische Halbinsel an der Atlantikküste, die Heimat des geheimnisvollen Filipe. Bei der Suche nach ihm gerät Katrin unversehens in ein Familiendrama. Und findet etwas, wonach sie gar nicht gesucht hat ...</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>978-3-442-49416-3</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Goldmann</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>03.05.2023</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>1. A.</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Breite 126 mm, Höhe 188 mm, Dicke 29 mmGewicht368 g</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Waldwissen</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>41.90</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Wohlleben, PeterIbisch, Pierre L.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>freizeit natur bestimmung</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Der Wald ist so viel mehr als Bäume! In ihrem ersten gemeinsamen Werk, das umfassend wie nie in die Geheimnisse des Waldes einführt, vereinen Deutschlands berühmtester Förster Peter Wohlleben und der renommierte Biologe Pierre L. Ibisch ihre herausragende Expertise und die neuesten Erkenntnisse der internationalen Wissenschaft. Sie bringen Licht ins Dickicht eines hoch komplexen Ökosystems. Anhand faszinierender Beispiele aus der Natur zeigen sie das ungeahnte Zusammenspiel der Pflanzen, Tiere, Mikroben, Viren, Pilze auf - eine Welt, in der kein Element ohne das andere existieren kann. Sie lassen uns den Wald erleben, wie wir ihn noch nicht kannten: als Supercomputer, Bioreaktor, Baumeister und Regenmacher. Auch wir Menschen sind Teil dieses fein austarierten Systems. Neueste wissenschaftliche Erkenntnisse geben aber auch Anlass, unseren Umgang mit dem Wald kritisch zu hinterfragen. Unsere Geschichte, unsere Kultur, unsere gesamte Entwicklung ist untrennbar mit dem Wald verbunden. Die Autoren zeigen, wie sehr nicht nur unsere Vergangenheit, sondern vor allem auch unsere Zukunft vom Wald abhängt. Doch wie können wir die Wälder bewirtschaften, ohne dabei unsere Lebensgrundlagen zu zerstören? Gemeinsam blicken die Waldexperten in die Zukunft des Waldes und damit in die Zukunft des Menschen, der ohne Wald nicht sein kann.
+Tiefe Einblicke in ein komplexes Ökosystem: geballtes Wissen, verblüffende Einsichten, ungeahnte ZusammenhängeDas umfassendste Buch zum Thema Wald - mit vielen Fotos, anschaulich und opulent bebildert
+Ausstattung: durchg. 4c</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>978-3-453-28149-3</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Ludwig</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>26.04.2023</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Breite 212 mm, Höhe 261 mm, Dicke 26 mmGewicht1108 g</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Allein</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Schreiber, Daniel</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>taschenbuch biografien</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Zu keiner Zeit haben so viele Menschen allein gelebt, und nie war elementarer zu spüren, wie schnell das selbstbestimmte Leben in Einsamkeit umschlagen kann. Aber kann man allein überhaupt glücklich sein? Und warum wird in einer Gesellschaft von Individualisten das Alleinleben als schambehaftetes Scheitern wahrgenommen?
+In seinem Bestseller ergründet Daniel Schreiber das Spannungsverhältnis zwischen dem Wunsch nach Rückzug und Freiheit und dem nach Nähe, Liebe und Gemeinschaft. Dabei greift er auf eigene Erfahrungen sowie philosophische und soziologische Ideen zurück. Ein »berauschend kluger Essay« (Denis Scheck) über die Frage, wie wir leben wollen.</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>978-3-518-47318-4</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Suhrkamp</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>17.04.2023</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Breite 116 mm, Höhe 188 mm, Dicke 14 mmGewicht154 g</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>55184198</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Das größte Glück im Leben</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>24.90</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Hauptmann, Gaby</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Töpferin Maike kämpft um ihre Existenz und ihr Elternhaus in Timmendorfer Strand
+Maike liebt ihr kleines, von Rosen umranktes Elternhaus in Timmendorfer Strand. Und obwohl es komisch klingt, fühlt sie, dass auch das Haus sie liebt. Seit ihrer Trennung lebt sie dort allein in einer idyllischen Sackgasse. Nicht ganz allein, denn mit ihren Nachbarn bildet sie eine verschworene Gemeinschaft. Bis ein Immobilienmakler ein Auge auf ihr Häuschen wirft - ihm ist jedes Mittel recht, um sein Ziel zu erreichen. Und er scheint zu wissen, dass Maike als Töpferin kaum Einnahmen hat ... Wie aus einem vermeintlichen Unglück Glück entstehen kann, erzählt niemand besser als Gaby Hauptmann!</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>978-3-492-06460-6</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Piper</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 205 mm, Dicke 32 mmGewicht452 g</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>55179762</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Ravenhall Academy 1: Verborgene Magie</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Kuhn, Julia</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>jugend junge_erwachsene</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>__Willkommen auf der Ravenhall Academy__
+Mit allem hätte Lilly Campbell gerechnet, aber nicht damit, dass sie eine Hexe ist: Von ihrer Grandma erfährt sie, dass uralte Magie in ihr schlummert - und um diese zu trainieren, soll sie die Ravenhall Academy besuchen. Zwischen Hexensprüchen, mystischen Legenden und sagenumwobenen Wesen muss sich Lilly nun in dieser neuen Welt zurechtfinden. Dabei gerät sie immer wieder mit dem leider viel zu attraktiven Jason aneinander, der ihr nicht mehr aus dem Kopf gehen will. Aber schon bald wird klar, dass auf Ravenhall nicht alles so ist, wie es scheint. Denn Lilly kommt einer dunklen Verschwörung auf die Spur, die das Erbe der Hexen tiefgreifend zu verändern droht ...
+Hol dir die wunderschön veredelte Liebhaberausgabe für dein Bücherregal, mit vierfarbigem Buchschnitt in der ersten Auflage!
+Persönliche Leseempfehlung von der Autorin Stefanie Hasse: »Eine romantische Academy-Geschichte in einem zauberhaften Setting, in dem man sich sofort zu Hause fühlt!«
+Julia Kuhn wurde 1996 in Süddeutschland geboren, wo sie auch heute noch mit ihrem Mann lebt. Wenn sie nicht gerade an neuen Geschichten schreibt, teilt sie Auf ihrem Instagram- und TikTok Account @july_reads Buchempfehlungen und erzählt über ihren Alltag als Autorin.
+//Dies ist der erste Band der magischen Romantasy-Dilogie »Ravenhall Academy«. Alle Romane der zauberhaften Academy-Fantasy:
+-- Band 1: Verborgene Magie
+-- Band 2: erscheint im Herbst 2023//
+Diese Reihe ist abgeschlossen.</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>978-3-551-30467-4</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Carlsen</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>27.04.2023</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>n-Nr.01</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Breite 136 mm, Höhe 215 mm, Dicke 34 mm</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Empusion</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>35.00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Tokarczuk, OlgaPalmes, LisaÜbersetzungQuinkenstein, LotharÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>September 1913, Görbersdorf in Niederschlesien. Inmitten von Bergen steht seit einem halben Jahrhundert das erste Sanatorium für Lungenkrankheiten. Mieczyslaw Wojnicz, Ingenieurstudent aus Lemberg, hofft, dass eine neuartige Behandlung und die kristallklare Luft des Kurorts seine Krankheit aufhalten, wenn nicht gar heilen werden. Die Diagnose allerdings gibt nur wenig Anlass zur Hoffnung: Schwindsucht. Mieczyslaw steigt in einem Gästehaus für Männer ab. Kranke aus ganz Europa versammeln sich dort, und wie auf Thomas Manns Zauberberg diskutieren und philosophieren sie unermüdlich miteinander - mit Vorliebe bei einem Gläschen Likör mit dem klingenden Namen »Schwärmerei«. Drängende Fragen treiben die Herren um: Wird es Krieg geben in Europa? Welche Staatsform ist die beste? Aber auch vermeintlich weniger drängende: Ob Dämonen existieren zum Beispiel oder ob man einem Text anmerkt, wer ihn verfasst hat - eine Frau oder ein Mann? Und mit der »Frauenfrage« befasst sich diese Herrenriege besonders gern. Auch bietet die kleine Welt von Görbersdorf reichlich Gesprächsstoff: Am Tag nach Mieczyslaws Ankunft hat die Frau des Pensionswirts Selbstmord begangen. Überhaupt komme es häufig zu mysteriösen Todesfällen in den Bergen ringsum, heißt es. Was Mieczyslaw nicht weiß: Dunkle Mächte haben es auch auf ihn abgesehen.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>978-3-311-10044-7</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 35 mmGewicht530 g</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>55771924</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Das Leuchten von Lavendel</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Luis, Hannah</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>taschenbuch romane</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Duftender Lavendel und die verführerischen Genüsse der Provence
+Mit einem ihrer selbst gebackenen Kuchen will Emilia ihren trauernden Großvater auf andere Gedanken bringen. Doch dann findet sie in seinem Keller einen alten Brief mit einer französischen Adresse und einem Herz aus Lavendelblüten, das den Namen Jette umrankt. Von einer Jette hat jedoch noch nie jemand aus der Familie gehört. Ihr Opa weigert sich, darüber zu sprechen. Also reist Emilia in die Provence, um nach der Unbekannten zu suchen. Sie hilft bei der Ernte auf der Lavendelfarm, auf der bereits ihr Großvater in jungen Jahren gearbeitet hat. Verzaubert vom magischen Licht und dem verführerischen Duft, kommt Emilia dem Rätsel des Lavendelherzens schließlich auf die Spur. Als sie dem attraktiven Besitzer der benachbarten Farm begegnet, muss sie sich jedoch fragen, warum ihr eigenes Herz plötzlich schneller schlägt.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>978-3-453-42737-2</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Heyne</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>11.05.2023</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Originalausgabe</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Breite 119 mm, Höhe 187 mm, Dicke 36 mmGewicht381 g</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Die Tote im Luganer See</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Vassena, Mascha</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Im beschaulichen Luganer See wird eine Leiche gefunden, und die Tote ist niemand Geringeres als die einst berühmte Chansonsängerin Livia. Doch wer hatte einen Grund, die alte, zurückgezogen lebende Dame zu töten? Wieder bitten Jugendliebe und Leiter der örtlichen Gerichtsmedizin Luca Cavadini und Ispettrice Moretti die Dolmetscherin Moira Rusconi bei dem Fall um Unterstützung. Die Ermittlungen führen sie in ein Geflecht aus dubiosen Geschäften, Rachegelüsten und Familiengeheimnissen. Und während ihr Vater Ambrogio sich in der Casa Rusconi mit ihrer anspruchsvollen Mutter abmüht, stellt Moira eigenmächtig Nachforschungen an und bringt sich dabei unwissentlich in Lebensgefahr.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>978-3-8479-0134-1</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Eichborn</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>28.04.2023</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>1. Aufl. 2023</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>n-Nr.02</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Schneetod</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>17.90</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Jónasson, RagnarAugustin, HelgaÜbersetzung</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>taschenbuch krimis</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>"Schneetod" ist der fünfte Band der Dark-Iceland-Serie von SPIEGEL-Bestseller-Autor Ragnar Jónasson.
+Ein verlassenes Haus am Ortsrand von SiglufjörÐur: Einer der beiden örtlichen Polizisten wird mitten in der Nacht kaltblütig ermordet. Warum war er um diese Uhrzeit dort draußen? Seinen Kollegen Ari trifft dieser Fall besonders. Und mit seinen Ermittlungen scheint er schlafende Hunde zu wecken, haben in diesem kleinen Ort dort mehr Leute etwas zu verbergen, als Ari geahnt hat. Nach und nach eröffnet sich ihm die ganze Tragödie eines menschlichen Lebens ...
+»Schneetod« ist der fünfte Band der Dark-Iceland-Serie von SPIEGEL-Bestseller-Autor Ragnar Jónasson.</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>978-3-442-77218-6</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Taschenbuch</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>btb</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>11.05.2023</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Neuveröffentlichung</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>n-Nr.05</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Damals im Tessin</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>26.90</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>belletristik krimi</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Zwanzig Jahre sind vergangen, seit Malvaglia, ein kleines Dorf in den Tessiner Bergen, geflutet wurde, um auf dem Gelände einen Stausee entstehen zu lassen. Beinahe haben die einstigen Bewohner, deren Häuser damals unter Wasser gesetzt wurden, das Unrecht vergessen. Besonders der verschlossene Privatdetektiv Elia Contini, der zurückgezogen in einem Häuschen in den Bergen wohnt und am liebsten durch die Wälder streift, um Füchse zu fotografieren, denkt ungern an die Zeit zurück, in der sein Vater unter ungeklärten Umständen verschwand. Doch jetzt soll der Stausee erweitert und jener Teil des Sees trockengelegt werden, auf dem auch das Haus seiner Kindheit stand. Alte Wunden brechen auf. Als kurz hintereinander der Bürgermeister und ein Ingenieur ermordet werden, gerät Contini ins Fadenkreuz der Ermittler. Um sich selbst zu entlasten, muss er sich endlich der Vergangenheit stellen und herausfinden, was damals wirklich geschah ...</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>978-3-7152-5503-3</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Atlantis Zürich</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 33 mmGewicht396 g</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>55771950</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Liebe oder Eierlikör - Fast eine Romanze</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>23.90</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Heldt, Dora</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>belletristik romane</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Früher war mehr Romantik ...
+Ernst Mannsen versteht die Welt nicht mehr. Die sonst so verlässliche Hilke Petersen trägt plötzlich Lippenstift und hat keine Zeit, auf dem Frühlingsbazar Kuchen zu verkaufen. Hella und Gudrun reden von Frühlingsgefühlen und Liebeshormonen und vermuten, dass Hilke eine Romanze hat. Und plötzlich taucht auch noch das Gerücht auf, dass das halbe Dorf sich bei einer Dating-App angemeldet hat, die Liebe oder Eierlikör heißt. Und das, obwohl Ernst schon so viel über Betrüger im Netz gelesen hat. Er vermutet, dass der Lippenstift nur der Anfang der Katastrophe ist, in die Hilke sich begibt, und ist entschlossen, das zu verhindern. Mithilfe seines Enkels Mats und Freundin Hella forscht er undercover nach, nicht ahnend, wie schnell man sich auf einem Date wiederfinden kann ...</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>978-3-423-28337-3</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Gebunden</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>DTV</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Breite 119 mm, Höhe 175 mm, Dicke 24 mmGewicht280 g</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Der Campingplatzkiller</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>25.90</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>belletristik schweizer</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Camping erfreut sich immer großerer Beliebtheit. Statt spießiger Kleinbürgeridylle ist das »Vanlife« auch in der jüngeren Generation angekommen: Ausgebuchte Platze, in der Hauptsaison sogar Wartelisten. Für die Dauercamper sind Touristen unerwünschte Eindringlinge in ihr Paradies. Heinrich »Henry« Kummer ist nicht ganz freiwillig auf dem Campingplatz gelandet. Mit 60 hat er seine Frühpensionierung beantragt - »So einen Bauchschuss lasst einen nachdenken«. Polizist war er, 32 Jahren lang. Aber keiner, der Verbrecher jagt, nicht einmal einer, der den Verkehr regelt. Als sich ihm die Gelegenheit geboten hat, ließ er sich in den Hausdienst versetzen. Und ist hangen geblieben. 25 Jahre hat er am Empfang des Kripo-Gebaudes in der Zürcher Kasernenstrasse verbracht. War für den Hausdienst zustandig, eine Art Abwart oder Portier. Und doch wurde ausgerechnet er bei einem Einsatz lebensgefahrlich verletzt. Aber auch das war keine Heldentat: Er war nur zur falschen Zeit am falschen Ort. Kummers neues Leben auf vier Radern beginnt weniger erholsam als gedacht: Dauercamperin Rosa wird tot in ihrem Wohnwagen gefunden: durchgeschnittene Kehle, ein einziger, sauberer Schnitt. Kummer ware nicht sein halbes Leben Polizist gewesen, wenn er den Ermittlungen tatenlos vom Campingstuhl aus zusehen würde ...</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>978-3-7152-5506-4</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Buch</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Paperback</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Atlantis Zürich</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>20.04.2023</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Deutsch</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Breite 125 mm, Höhe 205 mm, Dicke 25 mmGewicht270 g</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>55898510</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>